<commit_message>
Update model results for PR #6 (commit: c515db06af9749212396210ddb008160ca3489ae)
</commit_message>
<xml_diff>
--- a/optimal_team_2026.xlsx
+++ b/optimal_team_2026.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Starting Lineup" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bench" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Starting 22 (Onfield)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bench (8 Emergency)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Full Team" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Summary" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,24 +579,34 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
+          <t>overall_rank_score</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>objective</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>onfield</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0418</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Davis Sam</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -605,49 +615,49 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>20.89</v>
+        <v>24.07</v>
       </c>
       <c r="H2" t="n">
-        <v>13.02</v>
+        <v>15.95</v>
       </c>
       <c r="I2" t="n">
-        <v>7.87</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>5.36</v>
+        <v>7.96</v>
       </c>
       <c r="K2" t="n">
-        <v>6.16</v>
+        <v>6.65</v>
       </c>
       <c r="L2" t="n">
-        <v>0.44</v>
+        <v>0.16</v>
       </c>
       <c r="M2" t="n">
-        <v>0.27</v>
+        <v>1.08</v>
       </c>
       <c r="N2" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O2" t="n">
-        <v>98.55</v>
+        <v>116.78</v>
       </c>
       <c r="P2" t="n">
-        <v>631854</v>
+        <v>743313</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.2</v>
+        <v>1.05</v>
       </c>
       <c r="R2" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="S2" t="n">
-        <v>0.77</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -656,44 +666,50 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2" t="n">
-        <v>88.31</v>
+        <v>107.15</v>
       </c>
       <c r="X2" t="n">
-        <v>98.54219058106081</v>
+        <v>116.7800876450747</v>
       </c>
       <c r="Y2" t="n">
-        <v>15.59572157192339</v>
+        <v>15.71075544825325</v>
       </c>
       <c r="Z2" t="n">
         <v>1</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.2</v>
+        <v>1.3728</v>
       </c>
       <c r="AB2" t="n">
-        <v>18.71486588630807</v>
+        <v>21.56772507936206</v>
       </c>
       <c r="AC2" t="n">
-        <v>18.71486588630807</v>
+        <v>160.3157043191585</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>160.3157043191585</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0429</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Davis Jake</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -705,92 +721,98 @@
         <v>18</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>25.03</v>
+        <v>21.52</v>
       </c>
       <c r="H3" t="n">
-        <v>16.43</v>
+        <v>14.5</v>
       </c>
       <c r="I3" t="n">
-        <v>8.6</v>
+        <v>7.02</v>
       </c>
       <c r="J3" t="n">
-        <v>4.87</v>
+        <v>9.34</v>
       </c>
       <c r="K3" t="n">
-        <v>2.8</v>
+        <v>6.18</v>
       </c>
       <c r="L3" t="n">
-        <v>0.63</v>
+        <v>0.26</v>
       </c>
       <c r="M3" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="O3" t="n">
-        <v>96.29000000000001</v>
+        <v>112.9</v>
       </c>
       <c r="P3" t="n">
-        <v>654203</v>
+        <v>726852</v>
       </c>
       <c r="Q3" t="n">
         <v>1.3</v>
       </c>
       <c r="R3" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="S3" t="n">
-        <v>0.83</v>
+        <v>0.98</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" t="n">
-        <v>107.18</v>
+        <v>118.8</v>
       </c>
       <c r="X3" t="n">
-        <v>96.29227523422256</v>
+        <v>112.9002191479045</v>
       </c>
       <c r="Y3" t="n">
-        <v>14.7190207373281</v>
+        <v>15.53276583787408</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.3</v>
+        <v>2.206160000000001</v>
       </c>
       <c r="AB3" t="n">
-        <v>19.13472695852653</v>
+        <v>27.41421334470743</v>
       </c>
       <c r="AC3" t="n">
-        <v>19.13472695852653</v>
+        <v>199.2607579802729</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>199.2607579802729</v>
+      </c>
+      <c r="AE3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0087</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Smith Ben</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -799,49 +821,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G4" t="n">
-        <v>22.7</v>
+        <v>24.16</v>
       </c>
       <c r="H4" t="n">
-        <v>15.39</v>
+        <v>15.55</v>
       </c>
       <c r="I4" t="n">
-        <v>7.31</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>7.36</v>
       </c>
       <c r="K4" t="n">
-        <v>6.86</v>
+        <v>3.02</v>
       </c>
       <c r="L4" t="n">
-        <v>0.14</v>
+        <v>0.73</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6</v>
+        <v>0.72</v>
       </c>
       <c r="N4" t="n">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="O4" t="n">
-        <v>95.81</v>
+        <v>103.23</v>
       </c>
       <c r="P4" t="n">
-        <v>604863</v>
+        <v>678339</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R4" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="S4" t="n">
-        <v>0.86</v>
+        <v>0.97</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -850,44 +872,50 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>83.84999999999999</v>
+        <v>103.99</v>
       </c>
       <c r="X4" t="n">
-        <v>95.80921530620039</v>
+        <v>103.2308012602327</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.83982080342166</v>
+        <v>15.21817281038429</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.3</v>
+        <v>1.66221</v>
       </c>
       <c r="AB4" t="n">
-        <v>20.59176704444817</v>
+        <v>25.29579902714888</v>
       </c>
       <c r="AC4" t="n">
-        <v>20.59176704444817</v>
+        <v>171.5912701627714</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>171.5912701627714</v>
+      </c>
+      <c r="AE4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0234</t>
+          <t>P0244</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Davis Alex</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -899,46 +927,46 @@
         <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5" t="n">
-        <v>20.43</v>
+        <v>20.89</v>
       </c>
       <c r="H5" t="n">
-        <v>13.2</v>
+        <v>13.02</v>
       </c>
       <c r="I5" t="n">
-        <v>7.23</v>
+        <v>7.87</v>
       </c>
       <c r="J5" t="n">
-        <v>4.66</v>
+        <v>5.36</v>
       </c>
       <c r="K5" t="n">
-        <v>3.74</v>
+        <v>6.16</v>
       </c>
       <c r="L5" t="n">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
       <c r="M5" t="n">
-        <v>0.82</v>
+        <v>0.27</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="O5" t="n">
-        <v>84.90000000000001</v>
+        <v>98.55</v>
       </c>
       <c r="P5" t="n">
-        <v>555150</v>
+        <v>631854</v>
       </c>
       <c r="Q5" t="n">
         <v>1.2</v>
       </c>
       <c r="R5" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="S5" t="n">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -947,44 +975,50 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5" t="n">
-        <v>95.69</v>
+        <v>88.31</v>
       </c>
       <c r="X5" t="n">
-        <v>84.90018466025759</v>
+        <v>98.54839714106915</v>
       </c>
       <c r="Y5" t="n">
-        <v>15.29319727285555</v>
+        <v>15.59670384947617</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.2</v>
+        <v>1.6841</v>
       </c>
       <c r="AB5" t="n">
-        <v>18.35183672742666</v>
+        <v>26.26640895290281</v>
       </c>
       <c r="AC5" t="n">
-        <v>18.35183672742666</v>
+        <v>165.9653556252745</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>165.9653556252745</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0129</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Miller Dan</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -996,92 +1030,98 @@
         <v>18</v>
       </c>
       <c r="F6" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>18.28</v>
+        <v>25.03</v>
       </c>
       <c r="H6" t="n">
-        <v>11.12</v>
+        <v>16.43</v>
       </c>
       <c r="I6" t="n">
-        <v>7.16</v>
+        <v>8.6</v>
       </c>
       <c r="J6" t="n">
-        <v>6.37</v>
+        <v>4.87</v>
       </c>
       <c r="K6" t="n">
-        <v>1.89</v>
+        <v>2.8</v>
       </c>
       <c r="L6" t="n">
-        <v>0.34</v>
+        <v>0.63</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="N6" t="n">
-        <v>0.41</v>
+        <v>0.18</v>
       </c>
       <c r="O6" t="n">
-        <v>76.84</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P6" t="n">
-        <v>475343</v>
+        <v>654203</v>
       </c>
       <c r="Q6" t="n">
         <v>1.3</v>
       </c>
       <c r="R6" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="S6" t="n">
-        <v>0.58</v>
+        <v>0.83</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>62.77</v>
+        <v>107.18</v>
       </c>
       <c r="X6" t="n">
-        <v>76.84030364456702</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y6" t="n">
-        <v>16.1652330305836</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.3</v>
+        <v>1.8689</v>
       </c>
       <c r="AB6" t="n">
-        <v>18.91332264578281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC6" t="n">
-        <v>18.91332264578281</v>
+        <v>179.9564858710272</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>179.9564858710272</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0443</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taylor Ben</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1093,46 +1133,46 @@
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>22.69</v>
+        <v>22.7</v>
       </c>
       <c r="H7" t="n">
-        <v>13.75</v>
+        <v>15.39</v>
       </c>
       <c r="I7" t="n">
-        <v>8.94</v>
+        <v>7.31</v>
       </c>
       <c r="J7" t="n">
-        <v>2.14</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>1.27</v>
+        <v>6.86</v>
       </c>
       <c r="L7" t="n">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="M7" t="n">
         <v>0.6</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="O7" t="n">
-        <v>72.52</v>
+        <v>95.81</v>
       </c>
       <c r="P7" t="n">
-        <v>476223</v>
+        <v>604863</v>
       </c>
       <c r="Q7" t="n">
         <v>1.3</v>
       </c>
       <c r="R7" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="S7" t="n">
-        <v>0.43</v>
+        <v>0.86</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1141,44 +1181,50 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W7" t="n">
-        <v>59.52</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X7" t="n">
-        <v>72.52020676444907</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.22820333424658</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.3</v>
+        <v>1.8788</v>
       </c>
       <c r="AB7" t="n">
-        <v>19.79666433452055</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC7" t="n">
-        <v>19.79666433452055</v>
+        <v>180.0082776572042</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>180.0082776572042</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P0294</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Miller Alex</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1187,49 +1233,49 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>38.19</v>
+        <v>34.94</v>
       </c>
       <c r="H8" t="n">
-        <v>20.87</v>
+        <v>17.88</v>
       </c>
       <c r="I8" t="n">
-        <v>17.32</v>
+        <v>17.06</v>
       </c>
       <c r="J8" t="n">
-        <v>5.56</v>
+        <v>6.82</v>
       </c>
       <c r="K8" t="n">
-        <v>4.65</v>
+        <v>5.21</v>
       </c>
       <c r="L8" t="n">
-        <v>0.95</v>
+        <v>1.31</v>
       </c>
       <c r="M8" t="n">
-        <v>1.16</v>
+        <v>0.66</v>
       </c>
       <c r="N8" t="n">
-        <v>0.46</v>
+        <v>0.25</v>
       </c>
       <c r="O8" t="n">
-        <v>139.86</v>
+        <v>137.8</v>
       </c>
       <c r="P8" t="n">
         <v>800000</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R8" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="S8" t="n">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -1238,44 +1284,50 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W8" t="n">
-        <v>117.44</v>
+        <v>159.76</v>
       </c>
       <c r="X8" t="n">
-        <v>139.8609001310789</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y8" t="n">
-        <v>17.48261251638486</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z8" t="n">
         <v>1</v>
       </c>
       <c r="AA8" t="n">
-        <v>1</v>
+        <v>1.7336</v>
       </c>
       <c r="AB8" t="n">
-        <v>17.48261251638486</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC8" t="n">
-        <v>17.48261251638486</v>
+        <v>238.8896174134769</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>238.8896174134769</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0144</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Brown Jake</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1284,49 +1336,49 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>34.94</v>
+        <v>28.23</v>
       </c>
       <c r="H9" t="n">
-        <v>17.88</v>
+        <v>14.14</v>
       </c>
       <c r="I9" t="n">
-        <v>17.06</v>
+        <v>14.09</v>
       </c>
       <c r="J9" t="n">
-        <v>6.82</v>
+        <v>6.99</v>
       </c>
       <c r="K9" t="n">
-        <v>5.21</v>
+        <v>4.67</v>
       </c>
       <c r="L9" t="n">
-        <v>1.31</v>
+        <v>1.24</v>
       </c>
       <c r="M9" t="n">
-        <v>0.66</v>
+        <v>0.17</v>
       </c>
       <c r="N9" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="O9" t="n">
-        <v>137.8</v>
+        <v>118.13</v>
       </c>
       <c r="P9" t="n">
         <v>800000</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S9" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1335,28 +1387,34 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W9" t="n">
-        <v>159.76</v>
+        <v>133.15</v>
       </c>
       <c r="X9" t="n">
-        <v>137.7983922529015</v>
+        <v>118.1289308563486</v>
       </c>
       <c r="Y9" t="n">
-        <v>17.22479903161268</v>
+        <v>14.76611635704358</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.2</v>
+        <v>1.50535</v>
       </c>
       <c r="AB9" t="n">
-        <v>20.66975883793522</v>
+        <v>22.22817325807555</v>
       </c>
       <c r="AC9" t="n">
-        <v>20.66975883793522</v>
+        <v>177.8253860646044</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>177.8253860646044</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1438,38 +1496,44 @@
         <v>136.02</v>
       </c>
       <c r="X10" t="n">
-        <v>117.0899851234428</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.28913231302741</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z10" t="n">
         <v>0.9</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.3</v>
+        <v>1.8986</v>
       </c>
       <c r="AB10" t="n">
-        <v>17.88828480624207</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC10" t="n">
-        <v>17.88828480624207</v>
+        <v>200.0763702362455</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>200.0763702362455</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0306</t>
+          <t>P0152</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wilson Luke</t>
+          <t>Johnson Jake</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Melbourne</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1478,49 +1542,49 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="G11" t="n">
-        <v>25.67</v>
+        <v>26.72</v>
       </c>
       <c r="H11" t="n">
-        <v>13.82</v>
+        <v>13.54</v>
       </c>
       <c r="I11" t="n">
-        <v>11.85</v>
+        <v>13.18</v>
       </c>
       <c r="J11" t="n">
-        <v>5.22</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>5.21</v>
+        <v>3.74</v>
       </c>
       <c r="L11" t="n">
-        <v>1.41</v>
+        <v>0.45</v>
       </c>
       <c r="M11" t="n">
-        <v>0.57</v>
+        <v>1.11</v>
       </c>
       <c r="N11" t="n">
-        <v>0.71</v>
+        <v>0.47</v>
       </c>
       <c r="O11" t="n">
-        <v>111.38</v>
+        <v>111.83</v>
       </c>
       <c r="P11" t="n">
-        <v>689840</v>
+        <v>744081</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="R11" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1529,44 +1593,50 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W11" t="n">
-        <v>97.79000000000001</v>
+        <v>109.62</v>
       </c>
       <c r="X11" t="n">
-        <v>111.3798496674675</v>
+        <v>111.8296411589714</v>
       </c>
       <c r="Y11" t="n">
-        <v>16.14575114047713</v>
+        <v>15.02922950041345</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.2</v>
+        <v>1.5521</v>
       </c>
       <c r="AB11" t="n">
-        <v>19.37490136857256</v>
+        <v>23.32686710759172</v>
       </c>
       <c r="AC11" t="n">
-        <v>19.37490136857256</v>
+        <v>173.5707860428396</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>173.5707860428396</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0417</t>
+          <t>P0393</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Miller Matt</t>
+          <t>Miller Ben</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Carlton</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1575,49 +1645,49 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G12" t="n">
-        <v>31.5</v>
+        <v>24.49</v>
       </c>
       <c r="H12" t="n">
-        <v>16.29</v>
+        <v>14.26</v>
       </c>
       <c r="I12" t="n">
-        <v>15.22</v>
+        <v>10.24</v>
       </c>
       <c r="J12" t="n">
-        <v>7.12</v>
+        <v>7.25</v>
       </c>
       <c r="K12" t="n">
-        <v>1.77</v>
+        <v>5.77</v>
       </c>
       <c r="L12" t="n">
-        <v>0.32</v>
+        <v>0.38</v>
       </c>
       <c r="M12" t="n">
-        <v>0.66</v>
+        <v>0.79</v>
       </c>
       <c r="N12" t="n">
-        <v>0.58</v>
+        <v>0.5</v>
       </c>
       <c r="O12" t="n">
-        <v>110.91</v>
+        <v>111.67</v>
       </c>
       <c r="P12" t="n">
-        <v>713311</v>
+        <v>740105</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S12" t="n">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1626,44 +1696,50 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>125.7</v>
+        <v>107.67</v>
       </c>
       <c r="X12" t="n">
-        <v>110.9121967805699</v>
+        <v>111.6695204521162</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.54892561317152</v>
+        <v>15.08833482439873</v>
       </c>
       <c r="Z12" t="n">
         <v>1</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.3</v>
+        <v>1.65715</v>
       </c>
       <c r="AB12" t="n">
-        <v>20.21360329712298</v>
+        <v>25.00363405425236</v>
       </c>
       <c r="AC12" t="n">
-        <v>20.21360329712298</v>
+        <v>185.0531458172244</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>185.0531458172244</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P0373</t>
+          <t>P0306</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Johnson Jake</t>
+          <t>Wilson Luke</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1675,87 +1751,93 @@
         <v>19</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>33.36</v>
+        <v>25.67</v>
       </c>
       <c r="H13" t="n">
-        <v>17.54</v>
+        <v>13.82</v>
       </c>
       <c r="I13" t="n">
-        <v>15.82</v>
+        <v>11.85</v>
       </c>
       <c r="J13" t="n">
-        <v>0.47</v>
+        <v>5.22</v>
       </c>
       <c r="K13" t="n">
-        <v>4.3</v>
+        <v>5.21</v>
       </c>
       <c r="L13" t="n">
-        <v>0.71</v>
+        <v>1.41</v>
       </c>
       <c r="M13" t="n">
-        <v>0.08</v>
+        <v>0.57</v>
       </c>
       <c r="N13" t="n">
         <v>0.71</v>
       </c>
       <c r="O13" t="n">
-        <v>107.91</v>
+        <v>111.38</v>
       </c>
       <c r="P13" t="n">
-        <v>651832</v>
+        <v>689840</v>
       </c>
       <c r="Q13" t="n">
         <v>1.2</v>
       </c>
       <c r="R13" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="S13" t="n">
-        <v>0.84</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W13" t="n">
-        <v>100.75</v>
+        <v>97.79000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>107.9094756105358</v>
+        <v>111.3806294947733</v>
       </c>
       <c r="Y13" t="n">
-        <v>16.55479872275921</v>
+        <v>16.14586418514052</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.2</v>
+        <v>1.7402</v>
       </c>
       <c r="AB13" t="n">
-        <v>17.87918262057994</v>
+        <v>28.09703285498153</v>
       </c>
       <c r="AC13" t="n">
-        <v>17.87918262057994</v>
+        <v>193.8245714468046</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>193.8245714468046</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P0273</t>
+          <t>P0417</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Smith Jake</t>
+          <t>Miller Matt</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1772,46 +1854,46 @@
         <v>18</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>20.42</v>
+        <v>31.5</v>
       </c>
       <c r="H14" t="n">
-        <v>11.77</v>
+        <v>16.29</v>
       </c>
       <c r="I14" t="n">
-        <v>8.65</v>
+        <v>15.22</v>
       </c>
       <c r="J14" t="n">
-        <v>6.87</v>
+        <v>7.12</v>
       </c>
       <c r="K14" t="n">
-        <v>3.82</v>
+        <v>1.77</v>
       </c>
       <c r="L14" t="n">
-        <v>0.61</v>
+        <v>0.32</v>
       </c>
       <c r="M14" t="n">
-        <v>0.78</v>
+        <v>0.66</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>0.58</v>
       </c>
       <c r="O14" t="n">
-        <v>92.98</v>
+        <v>110.91</v>
       </c>
       <c r="P14" t="n">
-        <v>640806</v>
+        <v>713311</v>
       </c>
       <c r="Q14" t="n">
         <v>1.3</v>
       </c>
       <c r="R14" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="S14" t="n">
-        <v>0.63</v>
+        <v>0.93</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1820,44 +1902,50 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W14" t="n">
-        <v>97.06</v>
+        <v>125.7</v>
       </c>
       <c r="X14" t="n">
-        <v>92.98018685283391</v>
+        <v>110.9103823756901</v>
       </c>
       <c r="Y14" t="n">
-        <v>14.50988081460441</v>
+        <v>15.54867124938353</v>
       </c>
       <c r="Z14" t="n">
         <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.3</v>
+        <v>1.9019</v>
       </c>
       <c r="AB14" t="n">
-        <v>18.86284505898573</v>
+        <v>29.57201784920253</v>
       </c>
       <c r="AC14" t="n">
-        <v>18.86284505898573</v>
+        <v>210.9404562403251</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>210.9404562403251</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0371</t>
+          <t>P0263</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Anderson Dan</t>
+          <t>Taylor Alex</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Collingwood</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1866,49 +1954,49 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" t="n">
-        <v>23.24</v>
+        <v>28.97</v>
       </c>
       <c r="H15" t="n">
-        <v>12.75</v>
+        <v>14.86</v>
       </c>
       <c r="I15" t="n">
-        <v>10.49</v>
+        <v>14.11</v>
       </c>
       <c r="J15" t="n">
-        <v>1.26</v>
+        <v>6.97</v>
       </c>
       <c r="K15" t="n">
-        <v>5.83</v>
+        <v>3.58</v>
       </c>
       <c r="L15" t="n">
-        <v>0.44</v>
+        <v>0.18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="N15" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="O15" t="n">
-        <v>89.93000000000001</v>
+        <v>109.92</v>
       </c>
       <c r="P15" t="n">
-        <v>636733</v>
+        <v>680550</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.3</v>
+        <v>1.05</v>
       </c>
       <c r="R15" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="S15" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -1917,125 +2005,34 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W15" t="n">
-        <v>75.56</v>
+        <v>109.27</v>
       </c>
       <c r="X15" t="n">
-        <v>90.90976765942267</v>
+        <v>109.9206659296186</v>
       </c>
       <c r="Y15" t="n">
-        <v>14.27753354379664</v>
+        <v>16.15173990590237</v>
       </c>
       <c r="Z15" t="n">
         <v>1</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.3</v>
+        <v>1.58378</v>
       </c>
       <c r="AB15" t="n">
-        <v>18.56079360693564</v>
+        <v>25.58080262817006</v>
       </c>
       <c r="AC15" t="n">
-        <v>18.56079360693564</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>P0392</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Smith Jake</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Melbourne</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>RUC</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>18</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>17.67</v>
-      </c>
-      <c r="H16" t="n">
-        <v>9.56</v>
-      </c>
-      <c r="I16" t="n">
-        <v>8.109999999999999</v>
-      </c>
-      <c r="J16" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="K16" t="n">
-        <v>5.57</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N16" t="n">
-        <v>14.62</v>
-      </c>
-      <c r="O16" t="n">
-        <v>96.53</v>
-      </c>
-      <c r="P16" t="n">
-        <v>617323</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R16" t="n">
-        <v>30</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>1</v>
-      </c>
-      <c r="W16" t="n">
-        <v>100.61</v>
-      </c>
-      <c r="X16" t="n">
-        <v>96.52532869907621</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>15.63611410867183</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>20.32694834127338</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>20.32694834127338</v>
+        <v>174.0901522860113</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>174.0901522860113</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2046,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2200,7 +2197,17 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
+          <t>overall_rank_score</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>objective</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>onfield</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2366,24 +2373,34 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
+          <t>overall_rank_score</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>objective</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>onfield</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0418</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Davis Sam</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2392,49 +2409,49 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>20.89</v>
+        <v>24.07</v>
       </c>
       <c r="H2" t="n">
-        <v>13.02</v>
+        <v>15.95</v>
       </c>
       <c r="I2" t="n">
-        <v>7.87</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>5.36</v>
+        <v>7.96</v>
       </c>
       <c r="K2" t="n">
-        <v>6.16</v>
+        <v>6.65</v>
       </c>
       <c r="L2" t="n">
-        <v>0.44</v>
+        <v>0.16</v>
       </c>
       <c r="M2" t="n">
-        <v>0.27</v>
+        <v>1.08</v>
       </c>
       <c r="N2" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O2" t="n">
-        <v>98.55</v>
+        <v>116.78</v>
       </c>
       <c r="P2" t="n">
-        <v>631854</v>
+        <v>743313</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.2</v>
+        <v>1.05</v>
       </c>
       <c r="R2" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="S2" t="n">
-        <v>0.77</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -2443,44 +2460,50 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2" t="n">
-        <v>88.31</v>
+        <v>107.15</v>
       </c>
       <c r="X2" t="n">
-        <v>98.54219058106081</v>
+        <v>116.7800876450747</v>
       </c>
       <c r="Y2" t="n">
-        <v>15.59572157192339</v>
+        <v>15.71075544825325</v>
       </c>
       <c r="Z2" t="n">
         <v>1</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.2</v>
+        <v>1.3728</v>
       </c>
       <c r="AB2" t="n">
-        <v>18.71486588630807</v>
+        <v>21.56772507936206</v>
       </c>
       <c r="AC2" t="n">
-        <v>18.71486588630807</v>
+        <v>160.3157043191585</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>160.3157043191585</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0429</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Davis Jake</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2492,92 +2515,98 @@
         <v>18</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>25.03</v>
+        <v>21.52</v>
       </c>
       <c r="H3" t="n">
-        <v>16.43</v>
+        <v>14.5</v>
       </c>
       <c r="I3" t="n">
-        <v>8.6</v>
+        <v>7.02</v>
       </c>
       <c r="J3" t="n">
-        <v>4.87</v>
+        <v>9.34</v>
       </c>
       <c r="K3" t="n">
-        <v>2.8</v>
+        <v>6.18</v>
       </c>
       <c r="L3" t="n">
-        <v>0.63</v>
+        <v>0.26</v>
       </c>
       <c r="M3" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="O3" t="n">
-        <v>96.29000000000001</v>
+        <v>112.9</v>
       </c>
       <c r="P3" t="n">
-        <v>654203</v>
+        <v>726852</v>
       </c>
       <c r="Q3" t="n">
         <v>1.3</v>
       </c>
       <c r="R3" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="S3" t="n">
-        <v>0.83</v>
+        <v>0.98</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" t="n">
-        <v>107.18</v>
+        <v>118.8</v>
       </c>
       <c r="X3" t="n">
-        <v>96.29227523422256</v>
+        <v>112.9002191479045</v>
       </c>
       <c r="Y3" t="n">
-        <v>14.7190207373281</v>
+        <v>15.53276583787408</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.3</v>
+        <v>2.206160000000001</v>
       </c>
       <c r="AB3" t="n">
-        <v>19.13472695852653</v>
+        <v>27.41421334470743</v>
       </c>
       <c r="AC3" t="n">
-        <v>19.13472695852653</v>
+        <v>199.2607579802729</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>199.2607579802729</v>
+      </c>
+      <c r="AE3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0087</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Smith Ben</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2586,49 +2615,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G4" t="n">
-        <v>22.7</v>
+        <v>24.16</v>
       </c>
       <c r="H4" t="n">
-        <v>15.39</v>
+        <v>15.55</v>
       </c>
       <c r="I4" t="n">
-        <v>7.31</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>7.36</v>
       </c>
       <c r="K4" t="n">
-        <v>6.86</v>
+        <v>3.02</v>
       </c>
       <c r="L4" t="n">
-        <v>0.14</v>
+        <v>0.73</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6</v>
+        <v>0.72</v>
       </c>
       <c r="N4" t="n">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="O4" t="n">
-        <v>95.81</v>
+        <v>103.23</v>
       </c>
       <c r="P4" t="n">
-        <v>604863</v>
+        <v>678339</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R4" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="S4" t="n">
-        <v>0.86</v>
+        <v>0.97</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -2637,44 +2666,50 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>83.84999999999999</v>
+        <v>103.99</v>
       </c>
       <c r="X4" t="n">
-        <v>95.80921530620039</v>
+        <v>103.2308012602327</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.83982080342166</v>
+        <v>15.21817281038429</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.3</v>
+        <v>1.66221</v>
       </c>
       <c r="AB4" t="n">
-        <v>20.59176704444817</v>
+        <v>25.29579902714888</v>
       </c>
       <c r="AC4" t="n">
-        <v>20.59176704444817</v>
+        <v>171.5912701627714</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>171.5912701627714</v>
+      </c>
+      <c r="AE4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0234</t>
+          <t>P0244</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Davis Alex</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2686,46 +2721,46 @@
         <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5" t="n">
-        <v>20.43</v>
+        <v>20.89</v>
       </c>
       <c r="H5" t="n">
-        <v>13.2</v>
+        <v>13.02</v>
       </c>
       <c r="I5" t="n">
-        <v>7.23</v>
+        <v>7.87</v>
       </c>
       <c r="J5" t="n">
-        <v>4.66</v>
+        <v>5.36</v>
       </c>
       <c r="K5" t="n">
-        <v>3.74</v>
+        <v>6.16</v>
       </c>
       <c r="L5" t="n">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
       <c r="M5" t="n">
-        <v>0.82</v>
+        <v>0.27</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="O5" t="n">
-        <v>84.90000000000001</v>
+        <v>98.55</v>
       </c>
       <c r="P5" t="n">
-        <v>555150</v>
+        <v>631854</v>
       </c>
       <c r="Q5" t="n">
         <v>1.2</v>
       </c>
       <c r="R5" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="S5" t="n">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -2734,44 +2769,50 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5" t="n">
-        <v>95.69</v>
+        <v>88.31</v>
       </c>
       <c r="X5" t="n">
-        <v>84.90018466025759</v>
+        <v>98.54839714106915</v>
       </c>
       <c r="Y5" t="n">
-        <v>15.29319727285555</v>
+        <v>15.59670384947617</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.2</v>
+        <v>1.6841</v>
       </c>
       <c r="AB5" t="n">
-        <v>18.35183672742666</v>
+        <v>26.26640895290281</v>
       </c>
       <c r="AC5" t="n">
-        <v>18.35183672742666</v>
+        <v>165.9653556252745</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>165.9653556252745</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0129</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Miller Dan</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2783,92 +2824,98 @@
         <v>18</v>
       </c>
       <c r="F6" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>18.28</v>
+        <v>25.03</v>
       </c>
       <c r="H6" t="n">
-        <v>11.12</v>
+        <v>16.43</v>
       </c>
       <c r="I6" t="n">
-        <v>7.16</v>
+        <v>8.6</v>
       </c>
       <c r="J6" t="n">
-        <v>6.37</v>
+        <v>4.87</v>
       </c>
       <c r="K6" t="n">
-        <v>1.89</v>
+        <v>2.8</v>
       </c>
       <c r="L6" t="n">
-        <v>0.34</v>
+        <v>0.63</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="N6" t="n">
-        <v>0.41</v>
+        <v>0.18</v>
       </c>
       <c r="O6" t="n">
-        <v>76.84</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P6" t="n">
-        <v>475343</v>
+        <v>654203</v>
       </c>
       <c r="Q6" t="n">
         <v>1.3</v>
       </c>
       <c r="R6" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="S6" t="n">
-        <v>0.58</v>
+        <v>0.83</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>62.77</v>
+        <v>107.18</v>
       </c>
       <c r="X6" t="n">
-        <v>76.84030364456702</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y6" t="n">
-        <v>16.1652330305836</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.3</v>
+        <v>1.8689</v>
       </c>
       <c r="AB6" t="n">
-        <v>18.91332264578281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC6" t="n">
-        <v>18.91332264578281</v>
+        <v>179.9564858710272</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>179.9564858710272</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0443</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taylor Ben</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2880,46 +2927,46 @@
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>22.69</v>
+        <v>22.7</v>
       </c>
       <c r="H7" t="n">
-        <v>13.75</v>
+        <v>15.39</v>
       </c>
       <c r="I7" t="n">
-        <v>8.94</v>
+        <v>7.31</v>
       </c>
       <c r="J7" t="n">
-        <v>2.14</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>1.27</v>
+        <v>6.86</v>
       </c>
       <c r="L7" t="n">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="M7" t="n">
         <v>0.6</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="O7" t="n">
-        <v>72.52</v>
+        <v>95.81</v>
       </c>
       <c r="P7" t="n">
-        <v>476223</v>
+        <v>604863</v>
       </c>
       <c r="Q7" t="n">
         <v>1.3</v>
       </c>
       <c r="R7" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="S7" t="n">
-        <v>0.43</v>
+        <v>0.86</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -2928,44 +2975,50 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W7" t="n">
-        <v>59.52</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X7" t="n">
-        <v>72.52020676444907</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.22820333424658</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.3</v>
+        <v>1.8788</v>
       </c>
       <c r="AB7" t="n">
-        <v>19.79666433452055</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC7" t="n">
-        <v>19.79666433452055</v>
+        <v>180.0082776572042</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>180.0082776572042</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P0294</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Miller Alex</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2974,49 +3027,49 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>38.19</v>
+        <v>34.94</v>
       </c>
       <c r="H8" t="n">
-        <v>20.87</v>
+        <v>17.88</v>
       </c>
       <c r="I8" t="n">
-        <v>17.32</v>
+        <v>17.06</v>
       </c>
       <c r="J8" t="n">
-        <v>5.56</v>
+        <v>6.82</v>
       </c>
       <c r="K8" t="n">
-        <v>4.65</v>
+        <v>5.21</v>
       </c>
       <c r="L8" t="n">
-        <v>0.95</v>
+        <v>1.31</v>
       </c>
       <c r="M8" t="n">
-        <v>1.16</v>
+        <v>0.66</v>
       </c>
       <c r="N8" t="n">
-        <v>0.46</v>
+        <v>0.25</v>
       </c>
       <c r="O8" t="n">
-        <v>139.86</v>
+        <v>137.8</v>
       </c>
       <c r="P8" t="n">
         <v>800000</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R8" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="S8" t="n">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -3025,44 +3078,50 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W8" t="n">
-        <v>117.44</v>
+        <v>159.76</v>
       </c>
       <c r="X8" t="n">
-        <v>139.8609001310789</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y8" t="n">
-        <v>17.48261251638486</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z8" t="n">
         <v>1</v>
       </c>
       <c r="AA8" t="n">
-        <v>1</v>
+        <v>1.7336</v>
       </c>
       <c r="AB8" t="n">
-        <v>17.48261251638486</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC8" t="n">
-        <v>17.48261251638486</v>
+        <v>238.8896174134769</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>238.8896174134769</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0144</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Brown Jake</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3071,49 +3130,49 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>34.94</v>
+        <v>28.23</v>
       </c>
       <c r="H9" t="n">
-        <v>17.88</v>
+        <v>14.14</v>
       </c>
       <c r="I9" t="n">
-        <v>17.06</v>
+        <v>14.09</v>
       </c>
       <c r="J9" t="n">
-        <v>6.82</v>
+        <v>6.99</v>
       </c>
       <c r="K9" t="n">
-        <v>5.21</v>
+        <v>4.67</v>
       </c>
       <c r="L9" t="n">
-        <v>1.31</v>
+        <v>1.24</v>
       </c>
       <c r="M9" t="n">
-        <v>0.66</v>
+        <v>0.17</v>
       </c>
       <c r="N9" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="O9" t="n">
-        <v>137.8</v>
+        <v>118.13</v>
       </c>
       <c r="P9" t="n">
         <v>800000</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S9" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -3122,28 +3181,34 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W9" t="n">
-        <v>159.76</v>
+        <v>133.15</v>
       </c>
       <c r="X9" t="n">
-        <v>137.7983922529015</v>
+        <v>118.1289308563486</v>
       </c>
       <c r="Y9" t="n">
-        <v>17.22479903161268</v>
+        <v>14.76611635704358</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.2</v>
+        <v>1.50535</v>
       </c>
       <c r="AB9" t="n">
-        <v>20.66975883793522</v>
+        <v>22.22817325807555</v>
       </c>
       <c r="AC9" t="n">
-        <v>20.66975883793522</v>
+        <v>177.8253860646044</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>177.8253860646044</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -3225,38 +3290,44 @@
         <v>136.02</v>
       </c>
       <c r="X10" t="n">
-        <v>117.0899851234428</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.28913231302741</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z10" t="n">
         <v>0.9</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.3</v>
+        <v>1.8986</v>
       </c>
       <c r="AB10" t="n">
-        <v>17.88828480624207</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC10" t="n">
-        <v>17.88828480624207</v>
+        <v>200.0763702362455</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>200.0763702362455</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0306</t>
+          <t>P0152</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wilson Luke</t>
+          <t>Johnson Jake</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Melbourne</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3265,49 +3336,49 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="G11" t="n">
-        <v>25.67</v>
+        <v>26.72</v>
       </c>
       <c r="H11" t="n">
-        <v>13.82</v>
+        <v>13.54</v>
       </c>
       <c r="I11" t="n">
-        <v>11.85</v>
+        <v>13.18</v>
       </c>
       <c r="J11" t="n">
-        <v>5.22</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>5.21</v>
+        <v>3.74</v>
       </c>
       <c r="L11" t="n">
-        <v>1.41</v>
+        <v>0.45</v>
       </c>
       <c r="M11" t="n">
-        <v>0.57</v>
+        <v>1.11</v>
       </c>
       <c r="N11" t="n">
-        <v>0.71</v>
+        <v>0.47</v>
       </c>
       <c r="O11" t="n">
-        <v>111.38</v>
+        <v>111.83</v>
       </c>
       <c r="P11" t="n">
-        <v>689840</v>
+        <v>744081</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="R11" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -3316,44 +3387,50 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W11" t="n">
-        <v>97.79000000000001</v>
+        <v>109.62</v>
       </c>
       <c r="X11" t="n">
-        <v>111.3798496674675</v>
+        <v>111.8296411589714</v>
       </c>
       <c r="Y11" t="n">
-        <v>16.14575114047713</v>
+        <v>15.02922950041345</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.2</v>
+        <v>1.5521</v>
       </c>
       <c r="AB11" t="n">
-        <v>19.37490136857256</v>
+        <v>23.32686710759172</v>
       </c>
       <c r="AC11" t="n">
-        <v>19.37490136857256</v>
+        <v>173.5707860428396</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>173.5707860428396</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0417</t>
+          <t>P0393</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Miller Matt</t>
+          <t>Miller Ben</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Carlton</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3362,49 +3439,49 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G12" t="n">
-        <v>31.5</v>
+        <v>24.49</v>
       </c>
       <c r="H12" t="n">
-        <v>16.29</v>
+        <v>14.26</v>
       </c>
       <c r="I12" t="n">
-        <v>15.22</v>
+        <v>10.24</v>
       </c>
       <c r="J12" t="n">
-        <v>7.12</v>
+        <v>7.25</v>
       </c>
       <c r="K12" t="n">
-        <v>1.77</v>
+        <v>5.77</v>
       </c>
       <c r="L12" t="n">
-        <v>0.32</v>
+        <v>0.38</v>
       </c>
       <c r="M12" t="n">
-        <v>0.66</v>
+        <v>0.79</v>
       </c>
       <c r="N12" t="n">
-        <v>0.58</v>
+        <v>0.5</v>
       </c>
       <c r="O12" t="n">
-        <v>110.91</v>
+        <v>111.67</v>
       </c>
       <c r="P12" t="n">
-        <v>713311</v>
+        <v>740105</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S12" t="n">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -3413,44 +3490,50 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>125.7</v>
+        <v>107.67</v>
       </c>
       <c r="X12" t="n">
-        <v>110.9121967805699</v>
+        <v>111.6695204521162</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.54892561317152</v>
+        <v>15.08833482439873</v>
       </c>
       <c r="Z12" t="n">
         <v>1</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.3</v>
+        <v>1.65715</v>
       </c>
       <c r="AB12" t="n">
-        <v>20.21360329712298</v>
+        <v>25.00363405425236</v>
       </c>
       <c r="AC12" t="n">
-        <v>20.21360329712298</v>
+        <v>185.0531458172244</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>185.0531458172244</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P0373</t>
+          <t>P0306</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Johnson Jake</t>
+          <t>Wilson Luke</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3462,87 +3545,93 @@
         <v>19</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>33.36</v>
+        <v>25.67</v>
       </c>
       <c r="H13" t="n">
-        <v>17.54</v>
+        <v>13.82</v>
       </c>
       <c r="I13" t="n">
-        <v>15.82</v>
+        <v>11.85</v>
       </c>
       <c r="J13" t="n">
-        <v>0.47</v>
+        <v>5.22</v>
       </c>
       <c r="K13" t="n">
-        <v>4.3</v>
+        <v>5.21</v>
       </c>
       <c r="L13" t="n">
-        <v>0.71</v>
+        <v>1.41</v>
       </c>
       <c r="M13" t="n">
-        <v>0.08</v>
+        <v>0.57</v>
       </c>
       <c r="N13" t="n">
         <v>0.71</v>
       </c>
       <c r="O13" t="n">
-        <v>107.91</v>
+        <v>111.38</v>
       </c>
       <c r="P13" t="n">
-        <v>651832</v>
+        <v>689840</v>
       </c>
       <c r="Q13" t="n">
         <v>1.2</v>
       </c>
       <c r="R13" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="S13" t="n">
-        <v>0.84</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W13" t="n">
-        <v>100.75</v>
+        <v>97.79000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>107.9094756105358</v>
+        <v>111.3806294947733</v>
       </c>
       <c r="Y13" t="n">
-        <v>16.55479872275921</v>
+        <v>16.14586418514052</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.2</v>
+        <v>1.7402</v>
       </c>
       <c r="AB13" t="n">
-        <v>17.87918262057994</v>
+        <v>28.09703285498153</v>
       </c>
       <c r="AC13" t="n">
-        <v>17.87918262057994</v>
+        <v>193.8245714468046</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>193.8245714468046</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P0273</t>
+          <t>P0417</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Smith Jake</t>
+          <t>Miller Matt</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3559,46 +3648,46 @@
         <v>18</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>20.42</v>
+        <v>31.5</v>
       </c>
       <c r="H14" t="n">
-        <v>11.77</v>
+        <v>16.29</v>
       </c>
       <c r="I14" t="n">
-        <v>8.65</v>
+        <v>15.22</v>
       </c>
       <c r="J14" t="n">
-        <v>6.87</v>
+        <v>7.12</v>
       </c>
       <c r="K14" t="n">
-        <v>3.82</v>
+        <v>1.77</v>
       </c>
       <c r="L14" t="n">
-        <v>0.61</v>
+        <v>0.32</v>
       </c>
       <c r="M14" t="n">
-        <v>0.78</v>
+        <v>0.66</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>0.58</v>
       </c>
       <c r="O14" t="n">
-        <v>92.98</v>
+        <v>110.91</v>
       </c>
       <c r="P14" t="n">
-        <v>640806</v>
+        <v>713311</v>
       </c>
       <c r="Q14" t="n">
         <v>1.3</v>
       </c>
       <c r="R14" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="S14" t="n">
-        <v>0.63</v>
+        <v>0.93</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -3607,44 +3696,50 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W14" t="n">
-        <v>97.06</v>
+        <v>125.7</v>
       </c>
       <c r="X14" t="n">
-        <v>92.98018685283391</v>
+        <v>110.9103823756901</v>
       </c>
       <c r="Y14" t="n">
-        <v>14.50988081460441</v>
+        <v>15.54867124938353</v>
       </c>
       <c r="Z14" t="n">
         <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.3</v>
+        <v>1.9019</v>
       </c>
       <c r="AB14" t="n">
-        <v>18.86284505898573</v>
+        <v>29.57201784920253</v>
       </c>
       <c r="AC14" t="n">
-        <v>18.86284505898573</v>
+        <v>210.9404562403251</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>210.9404562403251</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0371</t>
+          <t>P0263</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Anderson Dan</t>
+          <t>Taylor Alex</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Collingwood</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -3653,49 +3748,49 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" t="n">
-        <v>23.24</v>
+        <v>28.97</v>
       </c>
       <c r="H15" t="n">
-        <v>12.75</v>
+        <v>14.86</v>
       </c>
       <c r="I15" t="n">
-        <v>10.49</v>
+        <v>14.11</v>
       </c>
       <c r="J15" t="n">
-        <v>1.26</v>
+        <v>6.97</v>
       </c>
       <c r="K15" t="n">
-        <v>5.83</v>
+        <v>3.58</v>
       </c>
       <c r="L15" t="n">
-        <v>0.44</v>
+        <v>0.18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="N15" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="O15" t="n">
-        <v>89.93000000000001</v>
+        <v>109.92</v>
       </c>
       <c r="P15" t="n">
-        <v>636733</v>
+        <v>680550</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.3</v>
+        <v>1.05</v>
       </c>
       <c r="R15" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="S15" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -3704,125 +3799,34 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W15" t="n">
-        <v>75.56</v>
+        <v>109.27</v>
       </c>
       <c r="X15" t="n">
-        <v>90.90976765942267</v>
+        <v>109.9206659296186</v>
       </c>
       <c r="Y15" t="n">
-        <v>14.27753354379664</v>
+        <v>16.15173990590237</v>
       </c>
       <c r="Z15" t="n">
         <v>1</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.3</v>
+        <v>1.58378</v>
       </c>
       <c r="AB15" t="n">
-        <v>18.56079360693564</v>
+        <v>25.58080262817006</v>
       </c>
       <c r="AC15" t="n">
-        <v>18.56079360693564</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>P0392</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Smith Jake</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Melbourne</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>RUC</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>18</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>17.67</v>
-      </c>
-      <c r="H16" t="n">
-        <v>9.56</v>
-      </c>
-      <c r="I16" t="n">
-        <v>8.109999999999999</v>
-      </c>
-      <c r="J16" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="K16" t="n">
-        <v>5.57</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N16" t="n">
-        <v>14.62</v>
-      </c>
-      <c r="O16" t="n">
-        <v>96.53</v>
-      </c>
-      <c r="P16" t="n">
-        <v>617323</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R16" t="n">
-        <v>30</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>1</v>
-      </c>
-      <c r="W16" t="n">
-        <v>100.61</v>
-      </c>
-      <c r="X16" t="n">
-        <v>96.52532869907621</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>15.63611410867183</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>20.32694834127338</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>20.32694834127338</v>
+        <v>174.0901522860113</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>174.0901522860113</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3836,7 +3840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3863,90 +3867,110 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total Cost</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>$9,713,319</t>
-        </is>
+          <t>Onfield Players</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Salary Cap</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>$10,000,000</t>
-        </is>
+          <t>Bench Players</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Remaining Budget</t>
+          <t>Total Cost</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$286,681</t>
+          <t>$9,973,149</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Starting 22 Predicted Score</t>
+          <t>Salary Cap</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1530.27</t>
+          <t>$10,000,000</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Average Player Value</t>
+          <t>Remaining Budget</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>19.12</t>
+          <t>$26,851</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Average Age</t>
+          <t>Starting 22 Predicted Score</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18.7</t>
+          <t>1552.29</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Average Player Value</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>26.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Average Age</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>19.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Average Injury History</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0.20</t>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix scipy version compatibility with Python 3.12
Co-authored-by: KingSoft69 <240275596+KingSoft69@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/optimal_team_2026.xlsx
+++ b/optimal_team_2026.xlsx
@@ -20,16 +20,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -437,157 +425,157 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>player_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>team</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>position</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>games_played</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>avg_disposals</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>avg_kicks</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>avg_handballs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>avg_marks</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>avg_tackles</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>avg_goals</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>avg_behinds</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>avg_hitouts</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>avg_score</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>potential</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>draft_pick</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>draft_value</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>injured_last_year</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>injury_history</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>games_last_3</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>form_last_5</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>predicted_score</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>value_score</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>risk_factor</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>upside_factor</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>adjusted_value</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>overall_rank_score</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>objective</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>onfield</t>
         </is>
@@ -2055,157 +2043,157 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>player_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>team</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>position</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>games_played</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>avg_disposals</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>avg_kicks</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>avg_handballs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>avg_marks</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>avg_tackles</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>avg_goals</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>avg_behinds</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>avg_hitouts</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>avg_score</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>potential</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>draft_pick</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>draft_value</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>injured_last_year</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>injury_history</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>games_last_3</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>form_last_5</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>predicted_score</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>value_score</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>risk_factor</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>upside_factor</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>adjusted_value</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>overall_rank_score</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>objective</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>onfield</t>
         </is>
@@ -2231,157 +2219,157 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>player_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>team</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>position</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>games_played</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>avg_disposals</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>avg_kicks</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>avg_handballs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>avg_marks</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>avg_tackles</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>avg_goals</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>avg_behinds</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>avg_hitouts</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>avg_score</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>potential</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>draft_pick</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>draft_value</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>injured_last_year</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>injury_history</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>games_last_3</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>form_last_5</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>predicted_score</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>value_score</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>risk_factor</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>upside_factor</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>adjusted_value</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>overall_rank_score</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>objective</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>onfield</t>
         </is>
@@ -3849,12 +3837,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>

</xml_diff>

<commit_message>
Fix team optimizer to properly allocate budget across all positions
Co-authored-by: KingSoft69 <240275596+KingSoft69@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/optimal_team_2026.xlsx
+++ b/optimal_team_2026.xlsx
@@ -584,17 +584,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P0418</t>
+          <t>P0429</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Davis Sam</t>
+          <t>Davis Jake</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -603,82 +603,82 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>24.07</v>
+        <v>21.52</v>
       </c>
       <c r="H2" t="n">
-        <v>15.95</v>
+        <v>14.5</v>
       </c>
       <c r="I2" t="n">
-        <v>8.119999999999999</v>
+        <v>7.02</v>
       </c>
       <c r="J2" t="n">
-        <v>7.96</v>
+        <v>9.34</v>
       </c>
       <c r="K2" t="n">
-        <v>6.65</v>
+        <v>6.18</v>
       </c>
       <c r="L2" t="n">
-        <v>0.16</v>
+        <v>0.26</v>
       </c>
       <c r="M2" t="n">
-        <v>1.08</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="O2" t="n">
-        <v>116.78</v>
+        <v>112.9</v>
       </c>
       <c r="P2" t="n">
-        <v>743313</v>
+        <v>726852</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.05</v>
+        <v>1.3</v>
       </c>
       <c r="R2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V2" t="n">
         <v>1</v>
       </c>
       <c r="W2" t="n">
-        <v>107.15</v>
+        <v>118.8</v>
       </c>
       <c r="X2" t="n">
-        <v>116.7800876450747</v>
+        <v>112.9002191479045</v>
       </c>
       <c r="Y2" t="n">
-        <v>15.71075544825325</v>
+        <v>15.53276583787408</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.3728</v>
+        <v>2.206160000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>21.56772507936206</v>
+        <v>27.41421334470743</v>
       </c>
       <c r="AC2" t="n">
-        <v>160.3157043191585</v>
+        <v>199.2607579802729</v>
       </c>
       <c r="AD2" t="n">
-        <v>160.3157043191585</v>
+        <v>199.2607579802729</v>
       </c>
       <c r="AE2" t="b">
         <v>1</v>
@@ -687,17 +687,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P0429</t>
+          <t>P0087</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Davis Jake</t>
+          <t>Smith Ben</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -706,82 +706,82 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>21.52</v>
+        <v>24.16</v>
       </c>
       <c r="H3" t="n">
-        <v>14.5</v>
+        <v>15.55</v>
       </c>
       <c r="I3" t="n">
-        <v>7.02</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>9.34</v>
+        <v>7.36</v>
       </c>
       <c r="K3" t="n">
-        <v>6.18</v>
+        <v>3.02</v>
       </c>
       <c r="L3" t="n">
-        <v>0.26</v>
+        <v>0.73</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="N3" t="n">
         <v>0.08</v>
       </c>
       <c r="O3" t="n">
-        <v>112.9</v>
+        <v>103.23</v>
       </c>
       <c r="P3" t="n">
-        <v>726852</v>
+        <v>678339</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S3" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>118.8</v>
+        <v>103.99</v>
       </c>
       <c r="X3" t="n">
-        <v>112.9002191479045</v>
+        <v>103.2308012602327</v>
       </c>
       <c r="Y3" t="n">
-        <v>15.53276583787408</v>
+        <v>15.21817281038429</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.206160000000001</v>
+        <v>1.66221</v>
       </c>
       <c r="AB3" t="n">
-        <v>27.41421334470743</v>
+        <v>25.29579902714888</v>
       </c>
       <c r="AC3" t="n">
-        <v>199.2607579802729</v>
+        <v>171.5912701627714</v>
       </c>
       <c r="AD3" t="n">
-        <v>199.2607579802729</v>
+        <v>171.5912701627714</v>
       </c>
       <c r="AE3" t="b">
         <v>1</v>
@@ -790,17 +790,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0087</t>
+          <t>P0244</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Smith Ben</t>
+          <t>Davis Alex</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -809,49 +809,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>24.16</v>
+        <v>20.89</v>
       </c>
       <c r="H4" t="n">
-        <v>15.55</v>
+        <v>13.02</v>
       </c>
       <c r="I4" t="n">
-        <v>8.609999999999999</v>
+        <v>7.87</v>
       </c>
       <c r="J4" t="n">
-        <v>7.36</v>
+        <v>5.36</v>
       </c>
       <c r="K4" t="n">
-        <v>3.02</v>
+        <v>6.16</v>
       </c>
       <c r="L4" t="n">
-        <v>0.73</v>
+        <v>0.44</v>
       </c>
       <c r="M4" t="n">
-        <v>0.72</v>
+        <v>0.27</v>
       </c>
       <c r="N4" t="n">
         <v>0.08</v>
       </c>
       <c r="O4" t="n">
-        <v>103.23</v>
+        <v>98.55</v>
       </c>
       <c r="P4" t="n">
-        <v>678339</v>
+        <v>631854</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R4" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="S4" t="n">
-        <v>0.97</v>
+        <v>0.77</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -860,31 +860,31 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W4" t="n">
-        <v>103.99</v>
+        <v>88.31</v>
       </c>
       <c r="X4" t="n">
-        <v>103.2308012602327</v>
+        <v>98.54839714106915</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.21817281038429</v>
+        <v>15.59670384947617</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.66221</v>
+        <v>1.6841</v>
       </c>
       <c r="AB4" t="n">
-        <v>25.29579902714888</v>
+        <v>26.26640895290281</v>
       </c>
       <c r="AC4" t="n">
-        <v>171.5912701627714</v>
+        <v>165.9653556252745</v>
       </c>
       <c r="AD4" t="n">
-        <v>171.5912701627714</v>
+        <v>165.9653556252745</v>
       </c>
       <c r="AE4" t="b">
         <v>1</v>
@@ -893,17 +893,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -912,49 +912,49 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>20.89</v>
+        <v>25.03</v>
       </c>
       <c r="H5" t="n">
-        <v>13.02</v>
+        <v>16.43</v>
       </c>
       <c r="I5" t="n">
-        <v>7.87</v>
+        <v>8.6</v>
       </c>
       <c r="J5" t="n">
-        <v>5.36</v>
+        <v>4.87</v>
       </c>
       <c r="K5" t="n">
-        <v>6.16</v>
+        <v>2.8</v>
       </c>
       <c r="L5" t="n">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="M5" t="n">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="N5" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O5" t="n">
-        <v>98.55</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>631854</v>
+        <v>654203</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R5" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S5" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -963,31 +963,31 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>88.31</v>
+        <v>107.18</v>
       </c>
       <c r="X5" t="n">
-        <v>98.54839714106915</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y5" t="n">
-        <v>15.59670384947617</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.6841</v>
+        <v>1.8689</v>
       </c>
       <c r="AB5" t="n">
-        <v>26.26640895290281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC5" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AD5" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AE5" t="b">
         <v>1</v>
@@ -996,17 +996,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1021,43 +1021,43 @@
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>25.03</v>
+        <v>22.7</v>
       </c>
       <c r="H6" t="n">
-        <v>16.43</v>
+        <v>15.39</v>
       </c>
       <c r="I6" t="n">
-        <v>8.6</v>
+        <v>7.31</v>
       </c>
       <c r="J6" t="n">
-        <v>4.87</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>2.8</v>
+        <v>6.86</v>
       </c>
       <c r="L6" t="n">
-        <v>0.63</v>
+        <v>0.14</v>
       </c>
       <c r="M6" t="n">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="N6" t="n">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="O6" t="n">
-        <v>96.29000000000001</v>
+        <v>95.81</v>
       </c>
       <c r="P6" t="n">
-        <v>654203</v>
+        <v>604863</v>
       </c>
       <c r="Q6" t="n">
         <v>1.3</v>
       </c>
       <c r="R6" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S6" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -1066,31 +1066,31 @@
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W6" t="n">
-        <v>107.18</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X6" t="n">
-        <v>96.29005611377129</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y6" t="n">
-        <v>14.71868152756427</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z6" t="n">
         <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.8689</v>
+        <v>1.8788</v>
       </c>
       <c r="AB6" t="n">
-        <v>27.50774390686487</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC6" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AD6" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AE6" t="b">
         <v>1</v>
@@ -1099,17 +1099,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0443</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Taylor Ben</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1121,46 +1121,46 @@
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>22.7</v>
+        <v>22.69</v>
       </c>
       <c r="H7" t="n">
-        <v>15.39</v>
+        <v>13.75</v>
       </c>
       <c r="I7" t="n">
-        <v>7.31</v>
+        <v>8.94</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>2.14</v>
       </c>
       <c r="K7" t="n">
-        <v>6.86</v>
+        <v>1.27</v>
       </c>
       <c r="L7" t="n">
-        <v>0.14</v>
+        <v>0.22</v>
       </c>
       <c r="M7" t="n">
         <v>0.6</v>
       </c>
       <c r="N7" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>95.81</v>
+        <v>72.52</v>
       </c>
       <c r="P7" t="n">
-        <v>604863</v>
+        <v>476223</v>
       </c>
       <c r="Q7" t="n">
         <v>1.3</v>
       </c>
       <c r="R7" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="S7" t="n">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1169,31 +1169,31 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7" t="n">
-        <v>83.84999999999999</v>
+        <v>59.52</v>
       </c>
       <c r="X7" t="n">
-        <v>95.81023933212911</v>
+        <v>72.51957248988509</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.83999010224284</v>
+        <v>15.22807014568492</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.8788</v>
+        <v>1.7369</v>
       </c>
       <c r="AB7" t="n">
-        <v>29.76017340409386</v>
+        <v>26.44963503604014</v>
       </c>
       <c r="AC7" t="n">
-        <v>180.0082776572042</v>
+        <v>125.9592454576814</v>
       </c>
       <c r="AD7" t="n">
-        <v>180.0082776572042</v>
+        <v>125.9592454576814</v>
       </c>
       <c r="AE7" t="b">
         <v>1</v>
@@ -1202,101 +1202,101 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0307</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Johnson Matt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E8" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" t="n">
         <v>19</v>
       </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
       <c r="G8" t="n">
-        <v>34.94</v>
+        <v>27.41</v>
       </c>
       <c r="H8" t="n">
-        <v>17.88</v>
+        <v>15.74</v>
       </c>
       <c r="I8" t="n">
-        <v>17.06</v>
+        <v>11.68</v>
       </c>
       <c r="J8" t="n">
-        <v>6.82</v>
+        <v>5.64</v>
       </c>
       <c r="K8" t="n">
-        <v>5.21</v>
+        <v>2.28</v>
       </c>
       <c r="L8" t="n">
-        <v>1.31</v>
+        <v>2.42</v>
       </c>
       <c r="M8" t="n">
         <v>0.66</v>
       </c>
       <c r="N8" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="O8" t="n">
-        <v>137.8</v>
+        <v>111.88</v>
       </c>
       <c r="P8" t="n">
-        <v>800000</v>
+        <v>697459</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R8" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="S8" t="n">
-        <v>0.92</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>159.76</v>
+        <v>122.87</v>
       </c>
       <c r="X8" t="n">
-        <v>137.7997331642114</v>
+        <v>111.8795752012058</v>
       </c>
       <c r="Y8" t="n">
-        <v>17.22496664552643</v>
+        <v>16.04102537944249</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.7336</v>
+        <v>1.8623</v>
       </c>
       <c r="AB8" t="n">
-        <v>29.86120217668461</v>
+        <v>26.88588140772217</v>
       </c>
       <c r="AC8" t="n">
-        <v>238.8896174134769</v>
+        <v>187.517999607485</v>
       </c>
       <c r="AD8" t="n">
-        <v>238.8896174134769</v>
+        <v>187.517999607485</v>
       </c>
       <c r="AE8" t="b">
         <v>1</v>
@@ -1305,68 +1305,68 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0144</t>
+          <t>P0116</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Brown Jake</t>
+          <t>Miller Sam</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>St Kilda</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G9" t="n">
-        <v>28.23</v>
+        <v>24.02</v>
       </c>
       <c r="H9" t="n">
-        <v>14.14</v>
+        <v>13.56</v>
       </c>
       <c r="I9" t="n">
-        <v>14.09</v>
+        <v>10.46</v>
       </c>
       <c r="J9" t="n">
-        <v>6.99</v>
+        <v>5.46</v>
       </c>
       <c r="K9" t="n">
-        <v>4.67</v>
+        <v>4.37</v>
       </c>
       <c r="L9" t="n">
-        <v>1.24</v>
+        <v>1.09</v>
       </c>
       <c r="M9" t="n">
-        <v>0.17</v>
+        <v>0.64</v>
       </c>
       <c r="N9" t="n">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="O9" t="n">
-        <v>118.13</v>
+        <v>102.95</v>
       </c>
       <c r="P9" t="n">
-        <v>800000</v>
+        <v>635441</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="R9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S9" t="n">
-        <v>0.95</v>
+        <v>0.84</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1378,28 +1378,28 @@
         <v>3</v>
       </c>
       <c r="W9" t="n">
-        <v>133.15</v>
+        <v>123.18</v>
       </c>
       <c r="X9" t="n">
-        <v>118.1289308563486</v>
+        <v>102.4889055369065</v>
       </c>
       <c r="Y9" t="n">
-        <v>14.76611635704358</v>
+        <v>16.12878387401922</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.50535</v>
+        <v>1.4168</v>
       </c>
       <c r="AB9" t="n">
-        <v>22.22817325807555</v>
+        <v>22.85126099271044</v>
       </c>
       <c r="AC9" t="n">
-        <v>177.8253860646044</v>
+        <v>145.2062813646891</v>
       </c>
       <c r="AD9" t="n">
-        <v>177.8253860646044</v>
+        <v>145.2062813646891</v>
       </c>
       <c r="AE9" t="b">
         <v>1</v>
@@ -1408,101 +1408,101 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P0197</t>
+          <t>P0284</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Davis Jack</t>
+          <t>Brown Ben</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Collingwood</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>31.59</v>
+        <v>20.7</v>
       </c>
       <c r="H10" t="n">
-        <v>17.64</v>
+        <v>11.77</v>
       </c>
       <c r="I10" t="n">
-        <v>13.95</v>
+        <v>8.94</v>
       </c>
       <c r="J10" t="n">
-        <v>4.82</v>
+        <v>7.93</v>
       </c>
       <c r="K10" t="n">
-        <v>4.92</v>
+        <v>3.81</v>
       </c>
       <c r="L10" t="n">
-        <v>0.11</v>
+        <v>1.59</v>
       </c>
       <c r="M10" t="n">
-        <v>0.51</v>
+        <v>0.57</v>
       </c>
       <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>102.34</v>
+      </c>
+      <c r="P10" t="n">
+        <v>662688</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="R10" t="n">
+        <v>5</v>
+      </c>
+      <c r="S10" t="n">
         <v>0.95</v>
       </c>
-      <c r="O10" t="n">
-        <v>117.09</v>
-      </c>
-      <c r="P10" t="n">
-        <v>765838</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R10" t="n">
-        <v>8</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.92</v>
-      </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
         <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>136.02</v>
+        <v>104.98</v>
       </c>
       <c r="X10" t="n">
-        <v>117.0900021280274</v>
+        <v>102.3404188393754</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.28913453341665</v>
+        <v>15.44322801067402</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.8986</v>
+        <v>1.815275</v>
       </c>
       <c r="AB10" t="n">
-        <v>26.12515574263037</v>
+        <v>28.03370572707628</v>
       </c>
       <c r="AC10" t="n">
-        <v>200.0763702362455</v>
+        <v>185.7760038086473</v>
       </c>
       <c r="AD10" t="n">
-        <v>200.0763702362455</v>
+        <v>185.7760038086473</v>
       </c>
       <c r="AE10" t="b">
         <v>1</v>
@@ -1511,17 +1511,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0152</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Johnson Jake</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1530,49 +1530,49 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>26.72</v>
+        <v>34.94</v>
       </c>
       <c r="H11" t="n">
-        <v>13.54</v>
+        <v>17.88</v>
       </c>
       <c r="I11" t="n">
-        <v>13.18</v>
+        <v>17.06</v>
       </c>
       <c r="J11" t="n">
-        <v>8.529999999999999</v>
+        <v>6.82</v>
       </c>
       <c r="K11" t="n">
-        <v>3.74</v>
+        <v>5.21</v>
       </c>
       <c r="L11" t="n">
-        <v>0.45</v>
+        <v>1.31</v>
       </c>
       <c r="M11" t="n">
-        <v>1.11</v>
+        <v>0.66</v>
       </c>
       <c r="N11" t="n">
-        <v>0.47</v>
+        <v>0.25</v>
       </c>
       <c r="O11" t="n">
-        <v>111.83</v>
+        <v>137.8</v>
       </c>
       <c r="P11" t="n">
-        <v>744081</v>
+        <v>800000</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R11" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="S11" t="n">
-        <v>0.87</v>
+        <v>0.92</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1584,28 +1584,28 @@
         <v>2</v>
       </c>
       <c r="W11" t="n">
-        <v>109.62</v>
+        <v>159.76</v>
       </c>
       <c r="X11" t="n">
-        <v>111.8296411589714</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y11" t="n">
-        <v>15.02922950041345</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.5521</v>
+        <v>1.7336</v>
       </c>
       <c r="AB11" t="n">
-        <v>23.32686710759172</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC11" t="n">
-        <v>173.5707860428396</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AD11" t="n">
-        <v>173.5707860428396</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AE11" t="b">
         <v>1</v>
@@ -1614,17 +1614,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0393</t>
+          <t>P0197</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Miller Ben</t>
+          <t>Davis Jack</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Carlton</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1633,82 +1633,82 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>24.49</v>
+        <v>31.59</v>
       </c>
       <c r="H12" t="n">
-        <v>14.26</v>
+        <v>17.64</v>
       </c>
       <c r="I12" t="n">
-        <v>10.24</v>
+        <v>13.95</v>
       </c>
       <c r="J12" t="n">
-        <v>7.25</v>
+        <v>4.82</v>
       </c>
       <c r="K12" t="n">
-        <v>5.77</v>
+        <v>4.92</v>
       </c>
       <c r="L12" t="n">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="M12" t="n">
-        <v>0.79</v>
+        <v>0.51</v>
       </c>
       <c r="N12" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="O12" t="n">
-        <v>111.67</v>
+        <v>117.09</v>
       </c>
       <c r="P12" t="n">
-        <v>740105</v>
+        <v>765838</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R12" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S12" t="n">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" t="n">
         <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>107.67</v>
+        <v>136.02</v>
       </c>
       <c r="X12" t="n">
-        <v>111.6695204521162</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.08833482439873</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z12" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.65715</v>
+        <v>1.8986</v>
       </c>
       <c r="AB12" t="n">
-        <v>25.00363405425236</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC12" t="n">
-        <v>185.0531458172244</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AD12" t="n">
-        <v>185.0531458172244</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AE12" t="b">
         <v>1</v>
@@ -1923,62 +1923,62 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0263</t>
+          <t>P0074</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Taylor Alex</t>
+          <t>Wilson Matt</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>North Melbourne</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>RUC</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>28.97</v>
+        <v>13.4</v>
       </c>
       <c r="H15" t="n">
-        <v>14.86</v>
+        <v>7.7</v>
       </c>
       <c r="I15" t="n">
-        <v>14.11</v>
+        <v>5.7</v>
       </c>
       <c r="J15" t="n">
-        <v>6.97</v>
+        <v>4.27</v>
       </c>
       <c r="K15" t="n">
-        <v>3.58</v>
+        <v>5.73</v>
       </c>
       <c r="L15" t="n">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
       <c r="M15" t="n">
-        <v>0.35</v>
+        <v>0.54</v>
       </c>
       <c r="N15" t="n">
-        <v>0.45</v>
+        <v>40.09</v>
       </c>
       <c r="O15" t="n">
-        <v>109.92</v>
+        <v>113.38</v>
       </c>
       <c r="P15" t="n">
-        <v>680550</v>
+        <v>741686</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.05</v>
+        <v>1.3</v>
       </c>
       <c r="R15" t="n">
         <v>4</v>
@@ -1993,31 +1993,31 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W15" t="n">
-        <v>109.27</v>
+        <v>99.53</v>
       </c>
       <c r="X15" t="n">
-        <v>109.9206659296186</v>
+        <v>113.3796228693182</v>
       </c>
       <c r="Y15" t="n">
-        <v>16.15173990590237</v>
+        <v>15.28674167630482</v>
       </c>
       <c r="Z15" t="n">
         <v>1</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.58378</v>
+        <v>2.19857</v>
       </c>
       <c r="AB15" t="n">
-        <v>25.58080262817006</v>
+        <v>33.6089716472735</v>
       </c>
       <c r="AC15" t="n">
-        <v>174.0901522860113</v>
+        <v>249.273037451797</v>
       </c>
       <c r="AD15" t="n">
-        <v>174.0901522860113</v>
+        <v>249.273037451797</v>
       </c>
       <c r="AE15" t="b">
         <v>1</v>
@@ -2034,7 +2034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2197,6 +2197,109 @@
         <is>
           <t>onfield</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P0052</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Johnson Ben</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>North Melbourne</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>FWD</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10.97</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="O2" t="n">
+        <v>55.31</v>
+      </c>
+      <c r="P2" t="n">
+        <v>345610</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>36</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>3</v>
+      </c>
+      <c r="W2" t="n">
+        <v>61.64</v>
+      </c>
+      <c r="X2" t="n">
+        <v>55.31062647898016</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>16.00376912675564</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1.642</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>26.27818890613276</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>90.82004867848543</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>90.82004867848543</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2210,7 +2313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2378,17 +2481,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P0418</t>
+          <t>P0429</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Davis Sam</t>
+          <t>Davis Jake</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Essendon</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2397,82 +2500,82 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>24.07</v>
+        <v>21.52</v>
       </c>
       <c r="H2" t="n">
-        <v>15.95</v>
+        <v>14.5</v>
       </c>
       <c r="I2" t="n">
-        <v>8.119999999999999</v>
+        <v>7.02</v>
       </c>
       <c r="J2" t="n">
-        <v>7.96</v>
+        <v>9.34</v>
       </c>
       <c r="K2" t="n">
-        <v>6.65</v>
+        <v>6.18</v>
       </c>
       <c r="L2" t="n">
-        <v>0.16</v>
+        <v>0.26</v>
       </c>
       <c r="M2" t="n">
-        <v>1.08</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="O2" t="n">
-        <v>116.78</v>
+        <v>112.9</v>
       </c>
       <c r="P2" t="n">
-        <v>743313</v>
+        <v>726852</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.05</v>
+        <v>1.3</v>
       </c>
       <c r="R2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V2" t="n">
         <v>1</v>
       </c>
       <c r="W2" t="n">
-        <v>107.15</v>
+        <v>118.8</v>
       </c>
       <c r="X2" t="n">
-        <v>116.7800876450747</v>
+        <v>112.9002191479045</v>
       </c>
       <c r="Y2" t="n">
-        <v>15.71075544825325</v>
+        <v>15.53276583787408</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.3728</v>
+        <v>2.206160000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>21.56772507936206</v>
+        <v>27.41421334470743</v>
       </c>
       <c r="AC2" t="n">
-        <v>160.3157043191585</v>
+        <v>199.2607579802729</v>
       </c>
       <c r="AD2" t="n">
-        <v>160.3157043191585</v>
+        <v>199.2607579802729</v>
       </c>
       <c r="AE2" t="b">
         <v>1</v>
@@ -2481,17 +2584,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P0429</t>
+          <t>P0087</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Davis Jake</t>
+          <t>Smith Ben</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2500,82 +2603,82 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>21.52</v>
+        <v>24.16</v>
       </c>
       <c r="H3" t="n">
-        <v>14.5</v>
+        <v>15.55</v>
       </c>
       <c r="I3" t="n">
-        <v>7.02</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>9.34</v>
+        <v>7.36</v>
       </c>
       <c r="K3" t="n">
-        <v>6.18</v>
+        <v>3.02</v>
       </c>
       <c r="L3" t="n">
-        <v>0.26</v>
+        <v>0.73</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="N3" t="n">
         <v>0.08</v>
       </c>
       <c r="O3" t="n">
-        <v>112.9</v>
+        <v>103.23</v>
       </c>
       <c r="P3" t="n">
-        <v>726852</v>
+        <v>678339</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="R3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S3" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>118.8</v>
+        <v>103.99</v>
       </c>
       <c r="X3" t="n">
-        <v>112.9002191479045</v>
+        <v>103.2308012602327</v>
       </c>
       <c r="Y3" t="n">
-        <v>15.53276583787408</v>
+        <v>15.21817281038429</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.206160000000001</v>
+        <v>1.66221</v>
       </c>
       <c r="AB3" t="n">
-        <v>27.41421334470743</v>
+        <v>25.29579902714888</v>
       </c>
       <c r="AC3" t="n">
-        <v>199.2607579802729</v>
+        <v>171.5912701627714</v>
       </c>
       <c r="AD3" t="n">
-        <v>199.2607579802729</v>
+        <v>171.5912701627714</v>
       </c>
       <c r="AE3" t="b">
         <v>1</v>
@@ -2584,17 +2687,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0087</t>
+          <t>P0244</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Smith Ben</t>
+          <t>Davis Alex</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2603,49 +2706,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>24.16</v>
+        <v>20.89</v>
       </c>
       <c r="H4" t="n">
-        <v>15.55</v>
+        <v>13.02</v>
       </c>
       <c r="I4" t="n">
-        <v>8.609999999999999</v>
+        <v>7.87</v>
       </c>
       <c r="J4" t="n">
-        <v>7.36</v>
+        <v>5.36</v>
       </c>
       <c r="K4" t="n">
-        <v>3.02</v>
+        <v>6.16</v>
       </c>
       <c r="L4" t="n">
-        <v>0.73</v>
+        <v>0.44</v>
       </c>
       <c r="M4" t="n">
-        <v>0.72</v>
+        <v>0.27</v>
       </c>
       <c r="N4" t="n">
         <v>0.08</v>
       </c>
       <c r="O4" t="n">
-        <v>103.23</v>
+        <v>98.55</v>
       </c>
       <c r="P4" t="n">
-        <v>678339</v>
+        <v>631854</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R4" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="S4" t="n">
-        <v>0.97</v>
+        <v>0.77</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -2654,31 +2757,31 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W4" t="n">
-        <v>103.99</v>
+        <v>88.31</v>
       </c>
       <c r="X4" t="n">
-        <v>103.2308012602327</v>
+        <v>98.54839714106915</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.21817281038429</v>
+        <v>15.59670384947617</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.66221</v>
+        <v>1.6841</v>
       </c>
       <c r="AB4" t="n">
-        <v>25.29579902714888</v>
+        <v>26.26640895290281</v>
       </c>
       <c r="AC4" t="n">
-        <v>171.5912701627714</v>
+        <v>165.9653556252745</v>
       </c>
       <c r="AD4" t="n">
-        <v>171.5912701627714</v>
+        <v>165.9653556252745</v>
       </c>
       <c r="AE4" t="b">
         <v>1</v>
@@ -2687,17 +2790,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2706,49 +2809,49 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>20.89</v>
+        <v>25.03</v>
       </c>
       <c r="H5" t="n">
-        <v>13.02</v>
+        <v>16.43</v>
       </c>
       <c r="I5" t="n">
-        <v>7.87</v>
+        <v>8.6</v>
       </c>
       <c r="J5" t="n">
-        <v>5.36</v>
+        <v>4.87</v>
       </c>
       <c r="K5" t="n">
-        <v>6.16</v>
+        <v>2.8</v>
       </c>
       <c r="L5" t="n">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="M5" t="n">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="N5" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O5" t="n">
-        <v>98.55</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>631854</v>
+        <v>654203</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R5" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S5" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -2757,31 +2860,31 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>88.31</v>
+        <v>107.18</v>
       </c>
       <c r="X5" t="n">
-        <v>98.54839714106915</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y5" t="n">
-        <v>15.59670384947617</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.6841</v>
+        <v>1.8689</v>
       </c>
       <c r="AB5" t="n">
-        <v>26.26640895290281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC5" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AD5" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AE5" t="b">
         <v>1</v>
@@ -2790,17 +2893,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2815,43 +2918,43 @@
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>25.03</v>
+        <v>22.7</v>
       </c>
       <c r="H6" t="n">
-        <v>16.43</v>
+        <v>15.39</v>
       </c>
       <c r="I6" t="n">
-        <v>8.6</v>
+        <v>7.31</v>
       </c>
       <c r="J6" t="n">
-        <v>4.87</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>2.8</v>
+        <v>6.86</v>
       </c>
       <c r="L6" t="n">
-        <v>0.63</v>
+        <v>0.14</v>
       </c>
       <c r="M6" t="n">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="N6" t="n">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="O6" t="n">
-        <v>96.29000000000001</v>
+        <v>95.81</v>
       </c>
       <c r="P6" t="n">
-        <v>654203</v>
+        <v>604863</v>
       </c>
       <c r="Q6" t="n">
         <v>1.3</v>
       </c>
       <c r="R6" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S6" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -2860,31 +2963,31 @@
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W6" t="n">
-        <v>107.18</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X6" t="n">
-        <v>96.29005611377129</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y6" t="n">
-        <v>14.71868152756427</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z6" t="n">
         <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.8689</v>
+        <v>1.8788</v>
       </c>
       <c r="AB6" t="n">
-        <v>27.50774390686487</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC6" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AD6" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AE6" t="b">
         <v>1</v>
@@ -2893,17 +2996,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0443</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Taylor Ben</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2915,46 +3018,46 @@
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>22.7</v>
+        <v>22.69</v>
       </c>
       <c r="H7" t="n">
-        <v>15.39</v>
+        <v>13.75</v>
       </c>
       <c r="I7" t="n">
-        <v>7.31</v>
+        <v>8.94</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>2.14</v>
       </c>
       <c r="K7" t="n">
-        <v>6.86</v>
+        <v>1.27</v>
       </c>
       <c r="L7" t="n">
-        <v>0.14</v>
+        <v>0.22</v>
       </c>
       <c r="M7" t="n">
         <v>0.6</v>
       </c>
       <c r="N7" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>95.81</v>
+        <v>72.52</v>
       </c>
       <c r="P7" t="n">
-        <v>604863</v>
+        <v>476223</v>
       </c>
       <c r="Q7" t="n">
         <v>1.3</v>
       </c>
       <c r="R7" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="S7" t="n">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -2963,31 +3066,31 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7" t="n">
-        <v>83.84999999999999</v>
+        <v>59.52</v>
       </c>
       <c r="X7" t="n">
-        <v>95.81023933212911</v>
+        <v>72.51957248988509</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.83999010224284</v>
+        <v>15.22807014568492</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.8788</v>
+        <v>1.7369</v>
       </c>
       <c r="AB7" t="n">
-        <v>29.76017340409386</v>
+        <v>26.44963503604014</v>
       </c>
       <c r="AC7" t="n">
-        <v>180.0082776572042</v>
+        <v>125.9592454576814</v>
       </c>
       <c r="AD7" t="n">
-        <v>180.0082776572042</v>
+        <v>125.9592454576814</v>
       </c>
       <c r="AE7" t="b">
         <v>1</v>
@@ -2996,101 +3099,101 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0307</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Johnson Matt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E8" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" t="n">
         <v>19</v>
       </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
       <c r="G8" t="n">
-        <v>34.94</v>
+        <v>27.41</v>
       </c>
       <c r="H8" t="n">
-        <v>17.88</v>
+        <v>15.74</v>
       </c>
       <c r="I8" t="n">
-        <v>17.06</v>
+        <v>11.68</v>
       </c>
       <c r="J8" t="n">
-        <v>6.82</v>
+        <v>5.64</v>
       </c>
       <c r="K8" t="n">
-        <v>5.21</v>
+        <v>2.28</v>
       </c>
       <c r="L8" t="n">
-        <v>1.31</v>
+        <v>2.42</v>
       </c>
       <c r="M8" t="n">
         <v>0.66</v>
       </c>
       <c r="N8" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="O8" t="n">
-        <v>137.8</v>
+        <v>111.88</v>
       </c>
       <c r="P8" t="n">
-        <v>800000</v>
+        <v>697459</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R8" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="S8" t="n">
-        <v>0.92</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>159.76</v>
+        <v>122.87</v>
       </c>
       <c r="X8" t="n">
-        <v>137.7997331642114</v>
+        <v>111.8795752012058</v>
       </c>
       <c r="Y8" t="n">
-        <v>17.22496664552643</v>
+        <v>16.04102537944249</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.7336</v>
+        <v>1.8623</v>
       </c>
       <c r="AB8" t="n">
-        <v>29.86120217668461</v>
+        <v>26.88588140772217</v>
       </c>
       <c r="AC8" t="n">
-        <v>238.8896174134769</v>
+        <v>187.517999607485</v>
       </c>
       <c r="AD8" t="n">
-        <v>238.8896174134769</v>
+        <v>187.517999607485</v>
       </c>
       <c r="AE8" t="b">
         <v>1</v>
@@ -3099,68 +3202,68 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0144</t>
+          <t>P0116</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Brown Jake</t>
+          <t>Miller Sam</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>St Kilda</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G9" t="n">
-        <v>28.23</v>
+        <v>24.02</v>
       </c>
       <c r="H9" t="n">
-        <v>14.14</v>
+        <v>13.56</v>
       </c>
       <c r="I9" t="n">
-        <v>14.09</v>
+        <v>10.46</v>
       </c>
       <c r="J9" t="n">
-        <v>6.99</v>
+        <v>5.46</v>
       </c>
       <c r="K9" t="n">
-        <v>4.67</v>
+        <v>4.37</v>
       </c>
       <c r="L9" t="n">
-        <v>1.24</v>
+        <v>1.09</v>
       </c>
       <c r="M9" t="n">
-        <v>0.17</v>
+        <v>0.64</v>
       </c>
       <c r="N9" t="n">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="O9" t="n">
-        <v>118.13</v>
+        <v>102.95</v>
       </c>
       <c r="P9" t="n">
-        <v>800000</v>
+        <v>635441</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="R9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="S9" t="n">
-        <v>0.95</v>
+        <v>0.84</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -3172,28 +3275,28 @@
         <v>3</v>
       </c>
       <c r="W9" t="n">
-        <v>133.15</v>
+        <v>123.18</v>
       </c>
       <c r="X9" t="n">
-        <v>118.1289308563486</v>
+        <v>102.4889055369065</v>
       </c>
       <c r="Y9" t="n">
-        <v>14.76611635704358</v>
+        <v>16.12878387401922</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.50535</v>
+        <v>1.4168</v>
       </c>
       <c r="AB9" t="n">
-        <v>22.22817325807555</v>
+        <v>22.85126099271044</v>
       </c>
       <c r="AC9" t="n">
-        <v>177.8253860646044</v>
+        <v>145.2062813646891</v>
       </c>
       <c r="AD9" t="n">
-        <v>177.8253860646044</v>
+        <v>145.2062813646891</v>
       </c>
       <c r="AE9" t="b">
         <v>1</v>
@@ -3202,101 +3305,101 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P0197</t>
+          <t>P0284</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Davis Jack</t>
+          <t>Brown Ben</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Collingwood</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>31.59</v>
+        <v>20.7</v>
       </c>
       <c r="H10" t="n">
-        <v>17.64</v>
+        <v>11.77</v>
       </c>
       <c r="I10" t="n">
-        <v>13.95</v>
+        <v>8.94</v>
       </c>
       <c r="J10" t="n">
-        <v>4.82</v>
+        <v>7.93</v>
       </c>
       <c r="K10" t="n">
-        <v>4.92</v>
+        <v>3.81</v>
       </c>
       <c r="L10" t="n">
-        <v>0.11</v>
+        <v>1.59</v>
       </c>
       <c r="M10" t="n">
-        <v>0.51</v>
+        <v>0.57</v>
       </c>
       <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>102.34</v>
+      </c>
+      <c r="P10" t="n">
+        <v>662688</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="R10" t="n">
+        <v>5</v>
+      </c>
+      <c r="S10" t="n">
         <v>0.95</v>
       </c>
-      <c r="O10" t="n">
-        <v>117.09</v>
-      </c>
-      <c r="P10" t="n">
-        <v>765838</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R10" t="n">
-        <v>8</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.92</v>
-      </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
         <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>136.02</v>
+        <v>104.98</v>
       </c>
       <c r="X10" t="n">
-        <v>117.0900021280274</v>
+        <v>102.3404188393754</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.28913453341665</v>
+        <v>15.44322801067402</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.8986</v>
+        <v>1.815275</v>
       </c>
       <c r="AB10" t="n">
-        <v>26.12515574263037</v>
+        <v>28.03370572707628</v>
       </c>
       <c r="AC10" t="n">
-        <v>200.0763702362455</v>
+        <v>185.7760038086473</v>
       </c>
       <c r="AD10" t="n">
-        <v>200.0763702362455</v>
+        <v>185.7760038086473</v>
       </c>
       <c r="AE10" t="b">
         <v>1</v>
@@ -3305,17 +3408,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0152</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Johnson Jake</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3324,49 +3427,49 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>26.72</v>
+        <v>34.94</v>
       </c>
       <c r="H11" t="n">
-        <v>13.54</v>
+        <v>17.88</v>
       </c>
       <c r="I11" t="n">
-        <v>13.18</v>
+        <v>17.06</v>
       </c>
       <c r="J11" t="n">
-        <v>8.529999999999999</v>
+        <v>6.82</v>
       </c>
       <c r="K11" t="n">
-        <v>3.74</v>
+        <v>5.21</v>
       </c>
       <c r="L11" t="n">
-        <v>0.45</v>
+        <v>1.31</v>
       </c>
       <c r="M11" t="n">
-        <v>1.11</v>
+        <v>0.66</v>
       </c>
       <c r="N11" t="n">
-        <v>0.47</v>
+        <v>0.25</v>
       </c>
       <c r="O11" t="n">
-        <v>111.83</v>
+        <v>137.8</v>
       </c>
       <c r="P11" t="n">
-        <v>744081</v>
+        <v>800000</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R11" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="S11" t="n">
-        <v>0.87</v>
+        <v>0.92</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -3378,28 +3481,28 @@
         <v>2</v>
       </c>
       <c r="W11" t="n">
-        <v>109.62</v>
+        <v>159.76</v>
       </c>
       <c r="X11" t="n">
-        <v>111.8296411589714</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y11" t="n">
-        <v>15.02922950041345</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.5521</v>
+        <v>1.7336</v>
       </c>
       <c r="AB11" t="n">
-        <v>23.32686710759172</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC11" t="n">
-        <v>173.5707860428396</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AD11" t="n">
-        <v>173.5707860428396</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AE11" t="b">
         <v>1</v>
@@ -3408,17 +3511,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0393</t>
+          <t>P0197</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Miller Ben</t>
+          <t>Davis Jack</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Carlton</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3427,82 +3530,82 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>24.49</v>
+        <v>31.59</v>
       </c>
       <c r="H12" t="n">
-        <v>14.26</v>
+        <v>17.64</v>
       </c>
       <c r="I12" t="n">
-        <v>10.24</v>
+        <v>13.95</v>
       </c>
       <c r="J12" t="n">
-        <v>7.25</v>
+        <v>4.82</v>
       </c>
       <c r="K12" t="n">
-        <v>5.77</v>
+        <v>4.92</v>
       </c>
       <c r="L12" t="n">
-        <v>0.38</v>
+        <v>0.11</v>
       </c>
       <c r="M12" t="n">
-        <v>0.79</v>
+        <v>0.51</v>
       </c>
       <c r="N12" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="O12" t="n">
-        <v>111.67</v>
+        <v>117.09</v>
       </c>
       <c r="P12" t="n">
-        <v>740105</v>
+        <v>765838</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R12" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S12" t="n">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" t="n">
         <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>107.67</v>
+        <v>136.02</v>
       </c>
       <c r="X12" t="n">
-        <v>111.6695204521162</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.08833482439873</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z12" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.65715</v>
+        <v>1.8986</v>
       </c>
       <c r="AB12" t="n">
-        <v>25.00363405425236</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC12" t="n">
-        <v>185.0531458172244</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AD12" t="n">
-        <v>185.0531458172244</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AE12" t="b">
         <v>1</v>
@@ -3717,62 +3820,62 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0263</t>
+          <t>P0074</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Taylor Alex</t>
+          <t>Wilson Matt</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Essendon</t>
+          <t>North Melbourne</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>RUC</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>28.97</v>
+        <v>13.4</v>
       </c>
       <c r="H15" t="n">
-        <v>14.86</v>
+        <v>7.7</v>
       </c>
       <c r="I15" t="n">
-        <v>14.11</v>
+        <v>5.7</v>
       </c>
       <c r="J15" t="n">
-        <v>6.97</v>
+        <v>4.27</v>
       </c>
       <c r="K15" t="n">
-        <v>3.58</v>
+        <v>5.73</v>
       </c>
       <c r="L15" t="n">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
       <c r="M15" t="n">
-        <v>0.35</v>
+        <v>0.54</v>
       </c>
       <c r="N15" t="n">
-        <v>0.45</v>
+        <v>40.09</v>
       </c>
       <c r="O15" t="n">
-        <v>109.92</v>
+        <v>113.38</v>
       </c>
       <c r="P15" t="n">
-        <v>680550</v>
+        <v>741686</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.05</v>
+        <v>1.3</v>
       </c>
       <c r="R15" t="n">
         <v>4</v>
@@ -3787,34 +3890,137 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
+        <v>1</v>
+      </c>
+      <c r="W15" t="n">
+        <v>99.53</v>
+      </c>
+      <c r="X15" t="n">
+        <v>113.3796228693182</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>15.28674167630482</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>2.19857</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>33.6089716472735</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>249.273037451797</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>249.273037451797</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P0052</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Johnson Ben</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>North Melbourne</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>FWD</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>18</v>
+      </c>
+      <c r="F16" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" t="n">
+        <v>10.97</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="O16" t="n">
+        <v>55.31</v>
+      </c>
+      <c r="P16" t="n">
+        <v>345610</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="R16" t="n">
+        <v>36</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
         <v>3</v>
       </c>
-      <c r="W15" t="n">
-        <v>109.27</v>
-      </c>
-      <c r="X15" t="n">
-        <v>109.9206659296186</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>16.15173990590237</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>1.58378</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>25.58080262817006</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>174.0901522860113</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>174.0901522860113</v>
-      </c>
-      <c r="AE15" t="b">
-        <v>1</v>
+      <c r="W16" t="n">
+        <v>61.64</v>
+      </c>
+      <c r="X16" t="n">
+        <v>55.31062647898016</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>16.00376912675564</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1.642</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>26.27818890613276</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>90.82004867848543</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>90.82004867848543</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3855,7 +4061,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -3875,7 +4081,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3886,7 +4092,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$9,973,149</t>
+          <t>$9,824,207</t>
         </is>
       </c>
     </row>
@@ -3910,7 +4116,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$26,851</t>
+          <t>$175,793</t>
         </is>
       </c>
     </row>
@@ -3922,7 +4128,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1552.29</t>
+          <t>1486.57</t>
         </is>
       </c>
     </row>
@@ -3934,7 +4140,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>26.26</t>
+          <t>27.60</t>
         </is>
       </c>
     </row>
@@ -3946,7 +4152,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19.9</t>
+          <t>18.9</t>
         </is>
       </c>
     </row>
@@ -3958,7 +4164,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve team selection algorithm with better budget management
Co-authored-by: KingSoft69 <240275596+KingSoft69@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/optimal_team_2026.xlsx
+++ b/optimal_team_2026.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,17 +790,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -809,49 +809,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>20.89</v>
+        <v>25.03</v>
       </c>
       <c r="H4" t="n">
-        <v>13.02</v>
+        <v>16.43</v>
       </c>
       <c r="I4" t="n">
-        <v>7.87</v>
+        <v>8.6</v>
       </c>
       <c r="J4" t="n">
-        <v>5.36</v>
+        <v>4.87</v>
       </c>
       <c r="K4" t="n">
-        <v>6.16</v>
+        <v>2.8</v>
       </c>
       <c r="L4" t="n">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="M4" t="n">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O4" t="n">
-        <v>98.55</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>631854</v>
+        <v>654203</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R4" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S4" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -860,31 +860,31 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>88.31</v>
+        <v>107.18</v>
       </c>
       <c r="X4" t="n">
-        <v>98.54839714106915</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.59670384947617</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.6841</v>
+        <v>1.8689</v>
       </c>
       <c r="AB4" t="n">
-        <v>26.26640895290281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC4" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AD4" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AE4" t="b">
         <v>1</v>
@@ -893,17 +893,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -918,43 +918,43 @@
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>25.03</v>
+        <v>22.7</v>
       </c>
       <c r="H5" t="n">
-        <v>16.43</v>
+        <v>15.39</v>
       </c>
       <c r="I5" t="n">
-        <v>8.6</v>
+        <v>7.31</v>
       </c>
       <c r="J5" t="n">
-        <v>4.87</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>2.8</v>
+        <v>6.86</v>
       </c>
       <c r="L5" t="n">
-        <v>0.63</v>
+        <v>0.14</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="N5" t="n">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="O5" t="n">
-        <v>96.29000000000001</v>
+        <v>95.81</v>
       </c>
       <c r="P5" t="n">
-        <v>654203</v>
+        <v>604863</v>
       </c>
       <c r="Q5" t="n">
         <v>1.3</v>
       </c>
       <c r="R5" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S5" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -963,31 +963,31 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W5" t="n">
-        <v>107.18</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X5" t="n">
-        <v>96.29005611377129</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y5" t="n">
-        <v>14.71868152756427</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.8689</v>
+        <v>1.8788</v>
       </c>
       <c r="AB5" t="n">
-        <v>27.50774390686487</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC5" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AD5" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AE5" t="b">
         <v>1</v>
@@ -996,17 +996,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0200</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Taylor Sam</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Geelong</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1015,82 +1015,82 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F6" t="n">
+        <v>93</v>
+      </c>
+      <c r="G6" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>11.41</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="O6" t="n">
+        <v>74.38</v>
+      </c>
+      <c r="P6" t="n">
+        <v>407688</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>50</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
         <v>2</v>
       </c>
-      <c r="G6" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="H6" t="n">
-        <v>15.39</v>
-      </c>
-      <c r="I6" t="n">
-        <v>7.31</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" t="n">
-        <v>6.86</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="O6" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="P6" t="n">
-        <v>604863</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R6" t="n">
-        <v>14</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
       <c r="V6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>83.84999999999999</v>
+        <v>69.97</v>
       </c>
       <c r="X6" t="n">
-        <v>95.81023933212911</v>
+        <v>74.37950322883475</v>
       </c>
       <c r="Y6" t="n">
-        <v>15.83999010224284</v>
+        <v>18.24422186300179</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.8788</v>
+        <v>1</v>
       </c>
       <c r="AB6" t="n">
-        <v>29.76017340409386</v>
+        <v>13.13583974136129</v>
       </c>
       <c r="AC6" t="n">
-        <v>180.0082776572042</v>
+        <v>53.55324232476103</v>
       </c>
       <c r="AD6" t="n">
-        <v>180.0082776572042</v>
+        <v>53.55324232476103</v>
       </c>
       <c r="AE6" t="b">
         <v>1</v>
@@ -1099,17 +1099,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0443</t>
+          <t>P0295</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taylor Ben</t>
+          <t>Taylor Jack</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>GWS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1118,49 +1118,49 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="G7" t="n">
-        <v>22.69</v>
+        <v>15.37</v>
       </c>
       <c r="H7" t="n">
-        <v>13.75</v>
+        <v>10.31</v>
       </c>
       <c r="I7" t="n">
-        <v>8.94</v>
+        <v>5.05</v>
       </c>
       <c r="J7" t="n">
-        <v>2.14</v>
+        <v>7.12</v>
       </c>
       <c r="K7" t="n">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M7" t="n">
         <v>0.22</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.6</v>
-      </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="O7" t="n">
-        <v>72.52</v>
+        <v>63.33</v>
       </c>
       <c r="P7" t="n">
-        <v>476223</v>
+        <v>436059</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.3</v>
+        <v>1.05</v>
       </c>
       <c r="R7" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S7" t="n">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1172,28 +1172,28 @@
         <v>2</v>
       </c>
       <c r="W7" t="n">
-        <v>59.52</v>
+        <v>56.88</v>
       </c>
       <c r="X7" t="n">
-        <v>72.51957248988509</v>
+        <v>63.32999763031351</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.22807014568492</v>
+        <v>14.52326351028496</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.7369</v>
+        <v>1.164</v>
       </c>
       <c r="AB7" t="n">
-        <v>26.44963503604014</v>
+        <v>16.9050787259717</v>
       </c>
       <c r="AC7" t="n">
-        <v>125.9592454576814</v>
+        <v>73.71611724168493</v>
       </c>
       <c r="AD7" t="n">
-        <v>125.9592454576814</v>
+        <v>73.71611724168493</v>
       </c>
       <c r="AE7" t="b">
         <v>1</v>
@@ -1305,68 +1305,68 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0116</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miller Sam</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>St Kilda</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>24.02</v>
+        <v>34.94</v>
       </c>
       <c r="H9" t="n">
-        <v>13.56</v>
+        <v>17.88</v>
       </c>
       <c r="I9" t="n">
-        <v>10.46</v>
+        <v>17.06</v>
       </c>
       <c r="J9" t="n">
-        <v>5.46</v>
+        <v>6.82</v>
       </c>
       <c r="K9" t="n">
-        <v>4.37</v>
+        <v>5.21</v>
       </c>
       <c r="L9" t="n">
-        <v>1.09</v>
+        <v>1.31</v>
       </c>
       <c r="M9" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="N9" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="O9" t="n">
-        <v>102.95</v>
+        <v>137.8</v>
       </c>
       <c r="P9" t="n">
-        <v>635441</v>
+        <v>800000</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R9" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="S9" t="n">
-        <v>0.84</v>
+        <v>0.92</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1375,31 +1375,31 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W9" t="n">
-        <v>123.18</v>
+        <v>159.76</v>
       </c>
       <c r="X9" t="n">
-        <v>102.4889055369065</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y9" t="n">
-        <v>16.12878387401922</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.4168</v>
+        <v>1.7336</v>
       </c>
       <c r="AB9" t="n">
-        <v>22.85126099271044</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC9" t="n">
-        <v>145.2062813646891</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AD9" t="n">
-        <v>145.2062813646891</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AE9" t="b">
         <v>1</v>
@@ -1408,101 +1408,101 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P0284</t>
+          <t>P0197</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Brown Ben</t>
+          <t>Davis Jack</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Collingwood</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>20.7</v>
+        <v>31.59</v>
       </c>
       <c r="H10" t="n">
-        <v>11.77</v>
+        <v>17.64</v>
       </c>
       <c r="I10" t="n">
-        <v>8.94</v>
+        <v>13.95</v>
       </c>
       <c r="J10" t="n">
-        <v>7.93</v>
+        <v>4.82</v>
       </c>
       <c r="K10" t="n">
-        <v>3.81</v>
+        <v>4.92</v>
       </c>
       <c r="L10" t="n">
-        <v>1.59</v>
+        <v>0.11</v>
       </c>
       <c r="M10" t="n">
-        <v>0.57</v>
+        <v>0.51</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="O10" t="n">
-        <v>102.34</v>
+        <v>117.09</v>
       </c>
       <c r="P10" t="n">
-        <v>662688</v>
+        <v>765838</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S10" t="n">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" t="n">
         <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>104.98</v>
+        <v>136.02</v>
       </c>
       <c r="X10" t="n">
-        <v>102.3404188393754</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.44322801067402</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z10" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.815275</v>
+        <v>1.8986</v>
       </c>
       <c r="AB10" t="n">
-        <v>28.03370572707628</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC10" t="n">
-        <v>185.7760038086473</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AD10" t="n">
-        <v>185.7760038086473</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AE10" t="b">
         <v>1</v>
@@ -1511,17 +1511,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0306</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Wilson Luke</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1536,43 +1536,43 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>34.94</v>
+        <v>25.67</v>
       </c>
       <c r="H11" t="n">
-        <v>17.88</v>
+        <v>13.82</v>
       </c>
       <c r="I11" t="n">
-        <v>17.06</v>
+        <v>11.85</v>
       </c>
       <c r="J11" t="n">
-        <v>6.82</v>
+        <v>5.22</v>
       </c>
       <c r="K11" t="n">
         <v>5.21</v>
       </c>
       <c r="L11" t="n">
-        <v>1.31</v>
+        <v>1.41</v>
       </c>
       <c r="M11" t="n">
-        <v>0.66</v>
+        <v>0.57</v>
       </c>
       <c r="N11" t="n">
-        <v>0.25</v>
+        <v>0.71</v>
       </c>
       <c r="O11" t="n">
-        <v>137.8</v>
+        <v>111.38</v>
       </c>
       <c r="P11" t="n">
-        <v>800000</v>
+        <v>689840</v>
       </c>
       <c r="Q11" t="n">
         <v>1.2</v>
       </c>
       <c r="R11" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S11" t="n">
-        <v>0.92</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1581,31 +1581,31 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W11" t="n">
-        <v>159.76</v>
+        <v>97.79000000000001</v>
       </c>
       <c r="X11" t="n">
-        <v>137.7997331642114</v>
+        <v>111.3806294947733</v>
       </c>
       <c r="Y11" t="n">
-        <v>17.22496664552643</v>
+        <v>16.14586418514052</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.7336</v>
+        <v>1.7402</v>
       </c>
       <c r="AB11" t="n">
-        <v>29.86120217668461</v>
+        <v>28.09703285498153</v>
       </c>
       <c r="AC11" t="n">
-        <v>238.8896174134769</v>
+        <v>193.8245714468046</v>
       </c>
       <c r="AD11" t="n">
-        <v>238.8896174134769</v>
+        <v>193.8245714468046</v>
       </c>
       <c r="AE11" t="b">
         <v>1</v>
@@ -1614,17 +1614,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0197</t>
+          <t>P0417</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Davis Jack</t>
+          <t>Miller Matt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1636,79 +1636,79 @@
         <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>31.59</v>
+        <v>31.5</v>
       </c>
       <c r="H12" t="n">
-        <v>17.64</v>
+        <v>16.29</v>
       </c>
       <c r="I12" t="n">
-        <v>13.95</v>
+        <v>15.22</v>
       </c>
       <c r="J12" t="n">
-        <v>4.82</v>
+        <v>7.12</v>
       </c>
       <c r="K12" t="n">
-        <v>4.92</v>
+        <v>1.77</v>
       </c>
       <c r="L12" t="n">
-        <v>0.11</v>
+        <v>0.32</v>
       </c>
       <c r="M12" t="n">
-        <v>0.51</v>
+        <v>0.66</v>
       </c>
       <c r="N12" t="n">
-        <v>0.95</v>
+        <v>0.58</v>
       </c>
       <c r="O12" t="n">
-        <v>117.09</v>
+        <v>110.91</v>
       </c>
       <c r="P12" t="n">
-        <v>765838</v>
+        <v>713311</v>
       </c>
       <c r="Q12" t="n">
         <v>1.3</v>
       </c>
       <c r="R12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S12" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W12" t="n">
-        <v>136.02</v>
+        <v>125.7</v>
       </c>
       <c r="X12" t="n">
-        <v>117.0900021280274</v>
+        <v>110.9103823756901</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.28913453341665</v>
+        <v>15.54867124938353</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.8986</v>
+        <v>1.9019</v>
       </c>
       <c r="AB12" t="n">
-        <v>26.12515574263037</v>
+        <v>29.57201784920253</v>
       </c>
       <c r="AC12" t="n">
-        <v>200.0763702362455</v>
+        <v>210.9404562403251</v>
       </c>
       <c r="AD12" t="n">
-        <v>200.0763702362455</v>
+        <v>210.9404562403251</v>
       </c>
       <c r="AE12" t="b">
         <v>1</v>
@@ -1717,17 +1717,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P0306</t>
+          <t>P0190</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Wilson Luke</t>
+          <t>Miller Tom</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1736,82 +1736,82 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G13" t="n">
-        <v>25.67</v>
+        <v>20.74</v>
       </c>
       <c r="H13" t="n">
-        <v>13.82</v>
+        <v>12.12</v>
       </c>
       <c r="I13" t="n">
-        <v>11.85</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="J13" t="n">
-        <v>5.22</v>
+        <v>3.89</v>
       </c>
       <c r="K13" t="n">
-        <v>5.21</v>
+        <v>2.4</v>
       </c>
       <c r="L13" t="n">
-        <v>1.41</v>
+        <v>0.99</v>
       </c>
       <c r="M13" t="n">
-        <v>0.57</v>
+        <v>0.26</v>
       </c>
       <c r="N13" t="n">
-        <v>0.71</v>
+        <v>0.64</v>
       </c>
       <c r="O13" t="n">
-        <v>111.38</v>
+        <v>81.72</v>
       </c>
       <c r="P13" t="n">
-        <v>689840</v>
+        <v>473239</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="S13" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>97.79000000000001</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>111.3806294947733</v>
+        <v>81.719637326624</v>
       </c>
       <c r="Y13" t="n">
-        <v>16.14586418514052</v>
+        <v>17.26815358130332</v>
       </c>
       <c r="Z13" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.7402</v>
+        <v>1</v>
       </c>
       <c r="AB13" t="n">
-        <v>28.09703285498153</v>
+        <v>13.81452286504265</v>
       </c>
       <c r="AC13" t="n">
-        <v>193.8245714468046</v>
+        <v>65.3757098612992</v>
       </c>
       <c r="AD13" t="n">
-        <v>193.8245714468046</v>
+        <v>65.3757098612992</v>
       </c>
       <c r="AE13" t="b">
         <v>1</v>
@@ -1820,17 +1820,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P0417</t>
+          <t>P0412</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Miller Matt</t>
+          <t>Davis Dan</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Geelong</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1839,49 +1839,49 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>31.5</v>
+        <v>18.88</v>
       </c>
       <c r="H14" t="n">
-        <v>16.29</v>
+        <v>10.54</v>
       </c>
       <c r="I14" t="n">
-        <v>15.22</v>
+        <v>8.34</v>
       </c>
       <c r="J14" t="n">
-        <v>7.12</v>
+        <v>5.56</v>
       </c>
       <c r="K14" t="n">
-        <v>1.77</v>
+        <v>1.09</v>
       </c>
       <c r="L14" t="n">
-        <v>0.32</v>
+        <v>0.51</v>
       </c>
       <c r="M14" t="n">
-        <v>0.66</v>
+        <v>0.02</v>
       </c>
       <c r="N14" t="n">
-        <v>0.58</v>
+        <v>0.4</v>
       </c>
       <c r="O14" t="n">
-        <v>110.91</v>
+        <v>72.83</v>
       </c>
       <c r="P14" t="n">
-        <v>713311</v>
+        <v>475823</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="S14" t="n">
-        <v>0.93</v>
+        <v>0.67</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1890,31 +1890,31 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>125.7</v>
+        <v>58.42</v>
       </c>
       <c r="X14" t="n">
-        <v>110.9103823756901</v>
+        <v>72.82985494070162</v>
       </c>
       <c r="Y14" t="n">
-        <v>15.54867124938353</v>
+        <v>15.30608124044059</v>
       </c>
       <c r="Z14" t="n">
         <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.9019</v>
+        <v>1.2474</v>
       </c>
       <c r="AB14" t="n">
-        <v>29.57201784920253</v>
+        <v>19.09280573932559</v>
       </c>
       <c r="AC14" t="n">
-        <v>210.9404562403251</v>
+        <v>90.84796105303121</v>
       </c>
       <c r="AD14" t="n">
-        <v>210.9404562403251</v>
+        <v>90.84796105303121</v>
       </c>
       <c r="AE14" t="b">
         <v>1</v>
@@ -1923,103 +1923,412 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0074</t>
+          <t>P0133</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wilson Matt</t>
+          <t>Smith Dan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>North Melbourne</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>RUC</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>18</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>13.4</v>
+        <v>19.33</v>
       </c>
       <c r="H15" t="n">
-        <v>7.7</v>
+        <v>9.91</v>
       </c>
       <c r="I15" t="n">
-        <v>5.7</v>
+        <v>9.43</v>
       </c>
       <c r="J15" t="n">
-        <v>4.27</v>
+        <v>4.56</v>
       </c>
       <c r="K15" t="n">
-        <v>5.73</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.42</v>
+        <v>1.11</v>
       </c>
       <c r="M15" t="n">
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
       <c r="N15" t="n">
-        <v>40.09</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>113.38</v>
+        <v>69.41</v>
       </c>
       <c r="P15" t="n">
-        <v>741686</v>
+        <v>466885</v>
       </c>
       <c r="Q15" t="n">
         <v>1.3</v>
       </c>
       <c r="R15" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="S15" t="n">
-        <v>0.96</v>
+        <v>0.68</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" t="n">
-        <v>99.53</v>
+        <v>74.33</v>
       </c>
       <c r="X15" t="n">
-        <v>113.3796228693182</v>
+        <v>69.40978572200886</v>
       </c>
       <c r="Y15" t="n">
-        <v>15.28674167630482</v>
+        <v>14.86657008085693</v>
       </c>
       <c r="Z15" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AA15" t="n">
-        <v>2.19857</v>
+        <v>1.8194</v>
       </c>
       <c r="AB15" t="n">
-        <v>33.6089716472735</v>
+        <v>18.93376632357777</v>
       </c>
       <c r="AC15" t="n">
-        <v>249.273037451797</v>
+        <v>88.39891489983606</v>
       </c>
       <c r="AD15" t="n">
-        <v>249.273037451797</v>
+        <v>88.39891489983606</v>
       </c>
       <c r="AE15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P0311</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Miller Alex</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Western Bulldogs</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>MID</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>25</v>
+      </c>
+      <c r="F16" t="n">
+        <v>27</v>
+      </c>
+      <c r="G16" t="n">
+        <v>13.88</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="I16" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="K16" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="P16" t="n">
+        <v>370794</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" t="n">
+        <v>59</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>2</v>
+      </c>
+      <c r="W16" t="n">
+        <v>58.76</v>
+      </c>
+      <c r="X16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>15.84437412902675</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>15.84437412902675</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P0142</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Wilson Alex</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Port Adelaide</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RUC</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>28</v>
+      </c>
+      <c r="F17" t="n">
+        <v>160</v>
+      </c>
+      <c r="G17" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="J17" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="O17" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="P17" t="n">
+        <v>428438</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>22</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>3</v>
+      </c>
+      <c r="W17" t="n">
+        <v>61.53</v>
+      </c>
+      <c r="X17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>16.26847641476558</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>16.26847641476558</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P0336</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Williams Matt</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GWS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RUC</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>29</v>
+      </c>
+      <c r="F18" t="n">
+        <v>96</v>
+      </c>
+      <c r="G18" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="I18" t="n">
+        <v>6.69</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N18" t="n">
+        <v>12.96</v>
+      </c>
+      <c r="O18" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="P18" t="n">
+        <v>446755</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="R18" t="n">
+        <v>48</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>2</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>58.33</v>
+      </c>
+      <c r="X18" t="n">
+        <v>67.69974680559991</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>15.1536629261228</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.7200000000000001</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>10.91063730680842</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>48.74381770003195</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>48.74381770003195</v>
+      </c>
+      <c r="AE18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2034,7 +2343,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2197,109 +2506,6 @@
         <is>
           <t>onfield</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>P0052</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Johnson Ben</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>North Melbourne</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>FWD</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>18</v>
-      </c>
-      <c r="F2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="H2" t="n">
-        <v>5.74</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5.22</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="O2" t="n">
-        <v>55.31</v>
-      </c>
-      <c r="P2" t="n">
-        <v>345610</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R2" t="n">
-        <v>36</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>3</v>
-      </c>
-      <c r="W2" t="n">
-        <v>61.64</v>
-      </c>
-      <c r="X2" t="n">
-        <v>55.31062647898016</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>16.00376912675564</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1.642</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>26.27818890613276</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>90.82004867848543</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>90.82004867848543</v>
-      </c>
-      <c r="AE2" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE16"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2687,17 +2893,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P0244</t>
+          <t>P0084</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Davis Alex</t>
+          <t>Williams Jack</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Fremantle</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2706,49 +2912,49 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>20.89</v>
+        <v>25.03</v>
       </c>
       <c r="H4" t="n">
-        <v>13.02</v>
+        <v>16.43</v>
       </c>
       <c r="I4" t="n">
-        <v>7.87</v>
+        <v>8.6</v>
       </c>
       <c r="J4" t="n">
-        <v>5.36</v>
+        <v>4.87</v>
       </c>
       <c r="K4" t="n">
-        <v>6.16</v>
+        <v>2.8</v>
       </c>
       <c r="L4" t="n">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
       <c r="M4" t="n">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="O4" t="n">
-        <v>98.55</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>631854</v>
+        <v>654203</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R4" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S4" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -2757,31 +2963,31 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>88.31</v>
+        <v>107.18</v>
       </c>
       <c r="X4" t="n">
-        <v>98.54839714106915</v>
+        <v>96.29005611377129</v>
       </c>
       <c r="Y4" t="n">
-        <v>15.59670384947617</v>
+        <v>14.71868152756427</v>
       </c>
       <c r="Z4" t="n">
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.6841</v>
+        <v>1.8689</v>
       </c>
       <c r="AB4" t="n">
-        <v>26.26640895290281</v>
+        <v>27.50774390686487</v>
       </c>
       <c r="AC4" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AD4" t="n">
-        <v>165.9653556252745</v>
+        <v>179.9564858710272</v>
       </c>
       <c r="AE4" t="b">
         <v>1</v>
@@ -2790,17 +2996,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P0084</t>
+          <t>P0340</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Williams Jack</t>
+          <t>Jones Alex</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fremantle</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2815,43 +3021,43 @@
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>25.03</v>
+        <v>22.7</v>
       </c>
       <c r="H5" t="n">
-        <v>16.43</v>
+        <v>15.39</v>
       </c>
       <c r="I5" t="n">
-        <v>8.6</v>
+        <v>7.31</v>
       </c>
       <c r="J5" t="n">
-        <v>4.87</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>2.8</v>
+        <v>6.86</v>
       </c>
       <c r="L5" t="n">
-        <v>0.63</v>
+        <v>0.14</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="N5" t="n">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="O5" t="n">
-        <v>96.29000000000001</v>
+        <v>95.81</v>
       </c>
       <c r="P5" t="n">
-        <v>654203</v>
+        <v>604863</v>
       </c>
       <c r="Q5" t="n">
         <v>1.3</v>
       </c>
       <c r="R5" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S5" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -2860,31 +3066,31 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W5" t="n">
-        <v>107.18</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="X5" t="n">
-        <v>96.29005611377129</v>
+        <v>95.81023933212911</v>
       </c>
       <c r="Y5" t="n">
-        <v>14.71868152756427</v>
+        <v>15.83999010224284</v>
       </c>
       <c r="Z5" t="n">
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.8689</v>
+        <v>1.8788</v>
       </c>
       <c r="AB5" t="n">
-        <v>27.50774390686487</v>
+        <v>29.76017340409386</v>
       </c>
       <c r="AC5" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AD5" t="n">
-        <v>179.9564858710272</v>
+        <v>180.0082776572042</v>
       </c>
       <c r="AE5" t="b">
         <v>1</v>
@@ -2893,17 +3099,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P0340</t>
+          <t>P0200</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jones Alex</t>
+          <t>Taylor Sam</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Geelong</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2912,82 +3118,82 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F6" t="n">
+        <v>93</v>
+      </c>
+      <c r="G6" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>11.41</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="O6" t="n">
+        <v>74.38</v>
+      </c>
+      <c r="P6" t="n">
+        <v>407688</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>50</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
         <v>2</v>
       </c>
-      <c r="G6" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="H6" t="n">
-        <v>15.39</v>
-      </c>
-      <c r="I6" t="n">
-        <v>7.31</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" t="n">
-        <v>6.86</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="O6" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="P6" t="n">
-        <v>604863</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="R6" t="n">
-        <v>14</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
       <c r="V6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>83.84999999999999</v>
+        <v>69.97</v>
       </c>
       <c r="X6" t="n">
-        <v>95.81023933212911</v>
+        <v>74.37950322883475</v>
       </c>
       <c r="Y6" t="n">
-        <v>15.83999010224284</v>
+        <v>18.24422186300179</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.8788</v>
+        <v>1</v>
       </c>
       <c r="AB6" t="n">
-        <v>29.76017340409386</v>
+        <v>13.13583974136129</v>
       </c>
       <c r="AC6" t="n">
-        <v>180.0082776572042</v>
+        <v>53.55324232476103</v>
       </c>
       <c r="AD6" t="n">
-        <v>180.0082776572042</v>
+        <v>53.55324232476103</v>
       </c>
       <c r="AE6" t="b">
         <v>1</v>
@@ -2996,17 +3202,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P0443</t>
+          <t>P0295</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Taylor Ben</t>
+          <t>Taylor Jack</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>GWS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3015,49 +3221,49 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="G7" t="n">
-        <v>22.69</v>
+        <v>15.37</v>
       </c>
       <c r="H7" t="n">
-        <v>13.75</v>
+        <v>10.31</v>
       </c>
       <c r="I7" t="n">
-        <v>8.94</v>
+        <v>5.05</v>
       </c>
       <c r="J7" t="n">
-        <v>2.14</v>
+        <v>7.12</v>
       </c>
       <c r="K7" t="n">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M7" t="n">
         <v>0.22</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.6</v>
-      </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="O7" t="n">
-        <v>72.52</v>
+        <v>63.33</v>
       </c>
       <c r="P7" t="n">
-        <v>476223</v>
+        <v>436059</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.3</v>
+        <v>1.05</v>
       </c>
       <c r="R7" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S7" t="n">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -3069,28 +3275,28 @@
         <v>2</v>
       </c>
       <c r="W7" t="n">
-        <v>59.52</v>
+        <v>56.88</v>
       </c>
       <c r="X7" t="n">
-        <v>72.51957248988509</v>
+        <v>63.32999763031351</v>
       </c>
       <c r="Y7" t="n">
-        <v>15.22807014568492</v>
+        <v>14.52326351028496</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.7369</v>
+        <v>1.164</v>
       </c>
       <c r="AB7" t="n">
-        <v>26.44963503604014</v>
+        <v>16.9050787259717</v>
       </c>
       <c r="AC7" t="n">
-        <v>125.9592454576814</v>
+        <v>73.71611724168493</v>
       </c>
       <c r="AD7" t="n">
-        <v>125.9592454576814</v>
+        <v>73.71611724168493</v>
       </c>
       <c r="AE7" t="b">
         <v>1</v>
@@ -3202,68 +3408,68 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P0116</t>
+          <t>P0187</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miller Sam</t>
+          <t>Miller Luke</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>St Kilda</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>24.02</v>
+        <v>34.94</v>
       </c>
       <c r="H9" t="n">
-        <v>13.56</v>
+        <v>17.88</v>
       </c>
       <c r="I9" t="n">
-        <v>10.46</v>
+        <v>17.06</v>
       </c>
       <c r="J9" t="n">
-        <v>5.46</v>
+        <v>6.82</v>
       </c>
       <c r="K9" t="n">
-        <v>4.37</v>
+        <v>5.21</v>
       </c>
       <c r="L9" t="n">
-        <v>1.09</v>
+        <v>1.31</v>
       </c>
       <c r="M9" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="N9" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="O9" t="n">
-        <v>102.95</v>
+        <v>137.8</v>
       </c>
       <c r="P9" t="n">
-        <v>635441</v>
+        <v>800000</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="R9" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="S9" t="n">
-        <v>0.84</v>
+        <v>0.92</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -3272,31 +3478,31 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W9" t="n">
-        <v>123.18</v>
+        <v>159.76</v>
       </c>
       <c r="X9" t="n">
-        <v>102.4889055369065</v>
+        <v>137.7997331642114</v>
       </c>
       <c r="Y9" t="n">
-        <v>16.12878387401922</v>
+        <v>17.22496664552643</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.4168</v>
+        <v>1.7336</v>
       </c>
       <c r="AB9" t="n">
-        <v>22.85126099271044</v>
+        <v>29.86120217668461</v>
       </c>
       <c r="AC9" t="n">
-        <v>145.2062813646891</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AD9" t="n">
-        <v>145.2062813646891</v>
+        <v>238.8896174134769</v>
       </c>
       <c r="AE9" t="b">
         <v>1</v>
@@ -3305,101 +3511,101 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P0284</t>
+          <t>P0197</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Brown Ben</t>
+          <t>Davis Jack</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Collingwood</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>20.7</v>
+        <v>31.59</v>
       </c>
       <c r="H10" t="n">
-        <v>11.77</v>
+        <v>17.64</v>
       </c>
       <c r="I10" t="n">
-        <v>8.94</v>
+        <v>13.95</v>
       </c>
       <c r="J10" t="n">
-        <v>7.93</v>
+        <v>4.82</v>
       </c>
       <c r="K10" t="n">
-        <v>3.81</v>
+        <v>4.92</v>
       </c>
       <c r="L10" t="n">
-        <v>1.59</v>
+        <v>0.11</v>
       </c>
       <c r="M10" t="n">
-        <v>0.57</v>
+        <v>0.51</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="O10" t="n">
-        <v>102.34</v>
+        <v>117.09</v>
       </c>
       <c r="P10" t="n">
-        <v>662688</v>
+        <v>765838</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S10" t="n">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" t="n">
         <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>104.98</v>
+        <v>136.02</v>
       </c>
       <c r="X10" t="n">
-        <v>102.3404188393754</v>
+        <v>117.0900021280274</v>
       </c>
       <c r="Y10" t="n">
-        <v>15.44322801067402</v>
+        <v>15.28913453341665</v>
       </c>
       <c r="Z10" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.815275</v>
+        <v>1.8986</v>
       </c>
       <c r="AB10" t="n">
-        <v>28.03370572707628</v>
+        <v>26.12515574263037</v>
       </c>
       <c r="AC10" t="n">
-        <v>185.7760038086473</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AD10" t="n">
-        <v>185.7760038086473</v>
+        <v>200.0763702362455</v>
       </c>
       <c r="AE10" t="b">
         <v>1</v>
@@ -3408,17 +3614,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P0187</t>
+          <t>P0306</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Miller Luke</t>
+          <t>Wilson Luke</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Hawthorn</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3433,43 +3639,43 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>34.94</v>
+        <v>25.67</v>
       </c>
       <c r="H11" t="n">
-        <v>17.88</v>
+        <v>13.82</v>
       </c>
       <c r="I11" t="n">
-        <v>17.06</v>
+        <v>11.85</v>
       </c>
       <c r="J11" t="n">
-        <v>6.82</v>
+        <v>5.22</v>
       </c>
       <c r="K11" t="n">
         <v>5.21</v>
       </c>
       <c r="L11" t="n">
-        <v>1.31</v>
+        <v>1.41</v>
       </c>
       <c r="M11" t="n">
-        <v>0.66</v>
+        <v>0.57</v>
       </c>
       <c r="N11" t="n">
-        <v>0.25</v>
+        <v>0.71</v>
       </c>
       <c r="O11" t="n">
-        <v>137.8</v>
+        <v>111.38</v>
       </c>
       <c r="P11" t="n">
-        <v>800000</v>
+        <v>689840</v>
       </c>
       <c r="Q11" t="n">
         <v>1.2</v>
       </c>
       <c r="R11" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S11" t="n">
-        <v>0.92</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -3478,31 +3684,31 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W11" t="n">
-        <v>159.76</v>
+        <v>97.79000000000001</v>
       </c>
       <c r="X11" t="n">
-        <v>137.7997331642114</v>
+        <v>111.3806294947733</v>
       </c>
       <c r="Y11" t="n">
-        <v>17.22496664552643</v>
+        <v>16.14586418514052</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.7336</v>
+        <v>1.7402</v>
       </c>
       <c r="AB11" t="n">
-        <v>29.86120217668461</v>
+        <v>28.09703285498153</v>
       </c>
       <c r="AC11" t="n">
-        <v>238.8896174134769</v>
+        <v>193.8245714468046</v>
       </c>
       <c r="AD11" t="n">
-        <v>238.8896174134769</v>
+        <v>193.8245714468046</v>
       </c>
       <c r="AE11" t="b">
         <v>1</v>
@@ -3511,17 +3717,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P0197</t>
+          <t>P0417</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Davis Jack</t>
+          <t>Miller Matt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Western Bulldogs</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3533,79 +3739,79 @@
         <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>31.59</v>
+        <v>31.5</v>
       </c>
       <c r="H12" t="n">
-        <v>17.64</v>
+        <v>16.29</v>
       </c>
       <c r="I12" t="n">
-        <v>13.95</v>
+        <v>15.22</v>
       </c>
       <c r="J12" t="n">
-        <v>4.82</v>
+        <v>7.12</v>
       </c>
       <c r="K12" t="n">
-        <v>4.92</v>
+        <v>1.77</v>
       </c>
       <c r="L12" t="n">
-        <v>0.11</v>
+        <v>0.32</v>
       </c>
       <c r="M12" t="n">
-        <v>0.51</v>
+        <v>0.66</v>
       </c>
       <c r="N12" t="n">
-        <v>0.95</v>
+        <v>0.58</v>
       </c>
       <c r="O12" t="n">
-        <v>117.09</v>
+        <v>110.91</v>
       </c>
       <c r="P12" t="n">
-        <v>765838</v>
+        <v>713311</v>
       </c>
       <c r="Q12" t="n">
         <v>1.3</v>
       </c>
       <c r="R12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S12" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W12" t="n">
-        <v>136.02</v>
+        <v>125.7</v>
       </c>
       <c r="X12" t="n">
-        <v>117.0900021280274</v>
+        <v>110.9103823756901</v>
       </c>
       <c r="Y12" t="n">
-        <v>15.28913453341665</v>
+        <v>15.54867124938353</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.8986</v>
+        <v>1.9019</v>
       </c>
       <c r="AB12" t="n">
-        <v>26.12515574263037</v>
+        <v>29.57201784920253</v>
       </c>
       <c r="AC12" t="n">
-        <v>200.0763702362455</v>
+        <v>210.9404562403251</v>
       </c>
       <c r="AD12" t="n">
-        <v>200.0763702362455</v>
+        <v>210.9404562403251</v>
       </c>
       <c r="AE12" t="b">
         <v>1</v>
@@ -3614,17 +3820,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P0306</t>
+          <t>P0190</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Wilson Luke</t>
+          <t>Miller Tom</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hawthorn</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3633,82 +3839,82 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G13" t="n">
-        <v>25.67</v>
+        <v>20.74</v>
       </c>
       <c r="H13" t="n">
-        <v>13.82</v>
+        <v>12.12</v>
       </c>
       <c r="I13" t="n">
-        <v>11.85</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="J13" t="n">
-        <v>5.22</v>
+        <v>3.89</v>
       </c>
       <c r="K13" t="n">
-        <v>5.21</v>
+        <v>2.4</v>
       </c>
       <c r="L13" t="n">
-        <v>1.41</v>
+        <v>0.99</v>
       </c>
       <c r="M13" t="n">
-        <v>0.57</v>
+        <v>0.26</v>
       </c>
       <c r="N13" t="n">
-        <v>0.71</v>
+        <v>0.64</v>
       </c>
       <c r="O13" t="n">
-        <v>111.38</v>
+        <v>81.72</v>
       </c>
       <c r="P13" t="n">
-        <v>689840</v>
+        <v>473239</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="S13" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>97.79000000000001</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>111.3806294947733</v>
+        <v>81.719637326624</v>
       </c>
       <c r="Y13" t="n">
-        <v>16.14586418514052</v>
+        <v>17.26815358130332</v>
       </c>
       <c r="Z13" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.7402</v>
+        <v>1</v>
       </c>
       <c r="AB13" t="n">
-        <v>28.09703285498153</v>
+        <v>13.81452286504265</v>
       </c>
       <c r="AC13" t="n">
-        <v>193.8245714468046</v>
+        <v>65.3757098612992</v>
       </c>
       <c r="AD13" t="n">
-        <v>193.8245714468046</v>
+        <v>65.3757098612992</v>
       </c>
       <c r="AE13" t="b">
         <v>1</v>
@@ -3717,17 +3923,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P0417</t>
+          <t>P0412</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Miller Matt</t>
+          <t>Davis Dan</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Port Adelaide</t>
+          <t>Geelong</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -3736,49 +3942,49 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>31.5</v>
+        <v>18.88</v>
       </c>
       <c r="H14" t="n">
-        <v>16.29</v>
+        <v>10.54</v>
       </c>
       <c r="I14" t="n">
-        <v>15.22</v>
+        <v>8.34</v>
       </c>
       <c r="J14" t="n">
-        <v>7.12</v>
+        <v>5.56</v>
       </c>
       <c r="K14" t="n">
-        <v>1.77</v>
+        <v>1.09</v>
       </c>
       <c r="L14" t="n">
-        <v>0.32</v>
+        <v>0.51</v>
       </c>
       <c r="M14" t="n">
-        <v>0.66</v>
+        <v>0.02</v>
       </c>
       <c r="N14" t="n">
-        <v>0.58</v>
+        <v>0.4</v>
       </c>
       <c r="O14" t="n">
-        <v>110.91</v>
+        <v>72.83</v>
       </c>
       <c r="P14" t="n">
-        <v>713311</v>
+        <v>475823</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="S14" t="n">
-        <v>0.93</v>
+        <v>0.67</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -3787,31 +3993,31 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>125.7</v>
+        <v>58.42</v>
       </c>
       <c r="X14" t="n">
-        <v>110.9103823756901</v>
+        <v>72.82985494070162</v>
       </c>
       <c r="Y14" t="n">
-        <v>15.54867124938353</v>
+        <v>15.30608124044059</v>
       </c>
       <c r="Z14" t="n">
         <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.9019</v>
+        <v>1.2474</v>
       </c>
       <c r="AB14" t="n">
-        <v>29.57201784920253</v>
+        <v>19.09280573932559</v>
       </c>
       <c r="AC14" t="n">
-        <v>210.9404562403251</v>
+        <v>90.84796105303121</v>
       </c>
       <c r="AD14" t="n">
-        <v>210.9404562403251</v>
+        <v>90.84796105303121</v>
       </c>
       <c r="AE14" t="b">
         <v>1</v>
@@ -3820,101 +4026,101 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P0074</t>
+          <t>P0133</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wilson Matt</t>
+          <t>Smith Dan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>North Melbourne</t>
+          <t>Port Adelaide</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>RUC</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>18</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>13.4</v>
+        <v>19.33</v>
       </c>
       <c r="H15" t="n">
-        <v>7.7</v>
+        <v>9.91</v>
       </c>
       <c r="I15" t="n">
-        <v>5.7</v>
+        <v>9.43</v>
       </c>
       <c r="J15" t="n">
-        <v>4.27</v>
+        <v>4.56</v>
       </c>
       <c r="K15" t="n">
-        <v>5.73</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.42</v>
+        <v>1.11</v>
       </c>
       <c r="M15" t="n">
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
       <c r="N15" t="n">
-        <v>40.09</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>113.38</v>
+        <v>69.41</v>
       </c>
       <c r="P15" t="n">
-        <v>741686</v>
+        <v>466885</v>
       </c>
       <c r="Q15" t="n">
         <v>1.3</v>
       </c>
       <c r="R15" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="S15" t="n">
-        <v>0.96</v>
+        <v>0.68</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" t="n">
-        <v>99.53</v>
+        <v>74.33</v>
       </c>
       <c r="X15" t="n">
-        <v>113.3796228693182</v>
+        <v>69.40978572200886</v>
       </c>
       <c r="Y15" t="n">
-        <v>15.28674167630482</v>
+        <v>14.86657008085693</v>
       </c>
       <c r="Z15" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AA15" t="n">
-        <v>2.19857</v>
+        <v>1.8194</v>
       </c>
       <c r="AB15" t="n">
-        <v>33.6089716472735</v>
+        <v>18.93376632357777</v>
       </c>
       <c r="AC15" t="n">
-        <v>249.273037451797</v>
+        <v>88.39891489983606</v>
       </c>
       <c r="AD15" t="n">
-        <v>249.273037451797</v>
+        <v>88.39891489983606</v>
       </c>
       <c r="AE15" t="b">
         <v>1</v>
@@ -3923,68 +4129,68 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>P0052</t>
+          <t>P0311</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Johnson Ben</t>
+          <t>Miller Alex</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>North Melbourne</t>
+          <t>Western Bulldogs</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F16" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G16" t="n">
-        <v>10.97</v>
+        <v>13.88</v>
       </c>
       <c r="H16" t="n">
-        <v>5.74</v>
+        <v>6.95</v>
       </c>
       <c r="I16" t="n">
-        <v>5.22</v>
+        <v>6.93</v>
       </c>
       <c r="J16" t="n">
-        <v>4.4</v>
+        <v>0.17</v>
       </c>
       <c r="K16" t="n">
-        <v>1.79</v>
+        <v>5.05</v>
       </c>
       <c r="L16" t="n">
-        <v>1.2</v>
+        <v>0.39</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="N16" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>55.31</v>
+        <v>58.75</v>
       </c>
       <c r="P16" t="n">
-        <v>345610</v>
+        <v>370794</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="R16" t="n">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="S16" t="n">
-        <v>0.64</v>
+        <v>0.41</v>
       </c>
       <c r="T16" t="n">
         <v>0</v>
@@ -3993,34 +4199,240 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
+        <v>2</v>
+      </c>
+      <c r="W16" t="n">
+        <v>58.76</v>
+      </c>
+      <c r="X16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>15.84437412902675</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>15.84437412902675</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>58.74998860798346</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P0142</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Wilson Alex</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Port Adelaide</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RUC</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>28</v>
+      </c>
+      <c r="F17" t="n">
+        <v>160</v>
+      </c>
+      <c r="G17" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="J17" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="O17" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="P17" t="n">
+        <v>428438</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>22</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
         <v>3</v>
       </c>
-      <c r="W16" t="n">
-        <v>61.64</v>
-      </c>
-      <c r="X16" t="n">
-        <v>55.31062647898016</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>16.00376912675564</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1.642</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>26.27818890613276</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>90.82004867848543</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>90.82004867848543</v>
-      </c>
-      <c r="AE16" t="b">
-        <v>0</v>
+      <c r="W17" t="n">
+        <v>61.53</v>
+      </c>
+      <c r="X17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>16.26847641476558</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>16.26847641476558</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>69.70033498189335</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P0336</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Williams Matt</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GWS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RUC</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>29</v>
+      </c>
+      <c r="F18" t="n">
+        <v>96</v>
+      </c>
+      <c r="G18" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="I18" t="n">
+        <v>6.69</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N18" t="n">
+        <v>12.96</v>
+      </c>
+      <c r="O18" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="P18" t="n">
+        <v>446755</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="R18" t="n">
+        <v>48</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>2</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>58.33</v>
+      </c>
+      <c r="X18" t="n">
+        <v>67.69974680559991</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>15.1536629261228</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.7200000000000001</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>10.91063730680842</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>48.74381770003195</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>48.74381770003195</v>
+      </c>
+      <c r="AE18" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4061,7 +4473,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -4071,7 +4483,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -4081,7 +4493,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -4092,7 +4504,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$9,824,207</t>
+          <t>$9,836,386</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4528,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$175,793</t>
+          <t>$163,614</t>
         </is>
       </c>
     </row>
@@ -4128,7 +4540,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1486.57</t>
+          <t>1555.11</t>
         </is>
       </c>
     </row>
@@ -4140,7 +4552,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27.60</t>
+          <t>22.08</t>
         </is>
       </c>
     </row>
@@ -4152,7 +4564,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18.9</t>
+          <t>21.3</t>
         </is>
       </c>
     </row>
@@ -4164,7 +4576,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>

</xml_diff>